<commit_message>
Fixed 2d4d code. Turned crossed-out values to 0 in Debrief_TG.
</commit_message>
<xml_diff>
--- a/raw-data-prep/raw_data/Debrief_TG.xlsx
+++ b/raw-data-prep/raw_data/Debrief_TG.xlsx
@@ -11,12 +11,15 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$R$125</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="152">
   <si>
     <t>Subject</t>
   </si>
@@ -112,9 +115,6 @@
   </si>
   <si>
     <t>To see if your partners response had any affect or punishment during the distraction test</t>
-  </si>
-  <si>
-    <t>mabye</t>
   </si>
   <si>
     <t>Depending on how the essay was graded we would probably decide how long the distractionwas. So if they gave a bad review it would cause a longer distraction</t>
@@ -182,9 +182,6 @@
     </r>
   </si>
   <si>
-    <t>nno</t>
-  </si>
-  <si>
     <t>to make it a surprise or unbiased</t>
   </si>
   <si>
@@ -245,9 +242,6 @@
     <t>to see how upset we were with each others grading</t>
   </si>
   <si>
-    <t>X-ed out</t>
-  </si>
-  <si>
     <t>Measuring aggression from video games and after "arguing" w/ someone of a different viewpoint</t>
   </si>
   <si>
@@ -260,15 +254,9 @@
     <t>To see if our writing topic had any effect</t>
   </si>
   <si>
-    <t>circle w/ slash</t>
-  </si>
-  <si>
     <t>To see if the evaluation of our essays affected how we treated our partner</t>
   </si>
   <si>
-    <t>0- N/A note</t>
-  </si>
-  <si>
     <t>So it could be random and because of any left over feelings from my essay grade</t>
   </si>
   <si>
@@ -402,9 +390,6 @@
   </si>
   <si>
     <t>I guess, dealing with different times of distraction. But why would the exoerimenter couldn't do that?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes </t>
   </si>
   <si>
     <r>
@@ -422,9 +407,6 @@
     </r>
   </si>
   <si>
-    <t>no (not very much)</t>
-  </si>
-  <si>
     <t>Because the video game may make me aggressive., so I may choose the longest time. But actually, the comments makes me feel not good very nuch</t>
   </si>
   <si>
@@ -446,12 +428,6 @@
     <t>N/a</t>
   </si>
   <si>
-    <t>XXXXX</t>
-  </si>
-  <si>
-    <t>XXXXXX</t>
-  </si>
-  <si>
     <t>Blank</t>
   </si>
   <si>
@@ -485,9 +461,6 @@
     <t>To measure nothing</t>
   </si>
   <si>
-    <t>`</t>
-  </si>
-  <si>
     <t>Perhaps to see how much we would distract the other person given the way they viewed the other's essay</t>
   </si>
   <si>
@@ -522,6 +495,21 @@
   </si>
   <si>
     <t>Game.affect.distraction</t>
+  </si>
+  <si>
+    <t>Maybe</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes </t>
   </si>
 </sst>
 </file>
@@ -912,10 +900,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:R125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:R1"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -967,7 +956,7 @@
         <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="P1" t="s">
         <v>14</v>
@@ -1023,10 +1012,10 @@
         <v>0</v>
       </c>
       <c r="O2" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="P2" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q2">
         <v>2</v>
@@ -1079,10 +1068,10 @@
         <v>0</v>
       </c>
       <c r="O3" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P3" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
       <c r="Q3">
         <v>2</v>
@@ -1091,7 +1080,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" hidden="1">
       <c r="A4">
         <v>185</v>
       </c>
@@ -1135,7 +1124,7 @@
         <v>0</v>
       </c>
       <c r="O4" t="s">
-        <v>22</v>
+        <v>147</v>
       </c>
       <c r="P4" t="s">
         <v>22</v>
@@ -1191,10 +1180,10 @@
         <v>1</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>24</v>
+        <v>150</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>24</v>
+        <v>150</v>
       </c>
       <c r="Q5" s="1">
         <v>3</v>
@@ -1247,10 +1236,10 @@
         <v>0</v>
       </c>
       <c r="O6" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P6" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="Q6">
         <v>4</v>
@@ -1303,10 +1292,10 @@
         <v>0</v>
       </c>
       <c r="O7" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P7" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q7">
         <v>3</v>
@@ -1359,10 +1348,10 @@
         <v>0</v>
       </c>
       <c r="O8" t="s">
-        <v>24</v>
+        <v>150</v>
       </c>
       <c r="P8" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q8">
         <v>4</v>
@@ -1371,7 +1360,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" hidden="1">
       <c r="A9">
         <v>190</v>
       </c>
@@ -1471,10 +1460,10 @@
         <v>0</v>
       </c>
       <c r="O10" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P10" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q10">
         <v>4</v>
@@ -1527,10 +1516,10 @@
         <v>1</v>
       </c>
       <c r="O11" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P11" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q11">
         <v>4</v>
@@ -1539,7 +1528,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" hidden="1">
       <c r="A12">
         <v>193</v>
       </c>
@@ -1583,7 +1572,7 @@
         <v>0</v>
       </c>
       <c r="O12" t="s">
-        <v>32</v>
+        <v>147</v>
       </c>
       <c r="P12" t="s">
         <v>18</v>
@@ -1592,7 +1581,7 @@
         <v>4</v>
       </c>
       <c r="R12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:18">
@@ -1639,19 +1628,19 @@
         <v>0</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="Q13" s="1">
         <v>2</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" hidden="1">
       <c r="A14">
         <v>195</v>
       </c>
@@ -1704,7 +1693,7 @@
         <v>4</v>
       </c>
       <c r="R14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:18">
@@ -1751,19 +1740,19 @@
         <v>0</v>
       </c>
       <c r="O15" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P15" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
       <c r="Q15">
         <v>1</v>
       </c>
       <c r="R15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" hidden="1">
       <c r="A16">
         <v>197</v>
       </c>
@@ -1816,10 +1805,10 @@
         <v>2</v>
       </c>
       <c r="R16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" hidden="1">
       <c r="A17">
         <v>199</v>
       </c>
@@ -1872,7 +1861,7 @@
         <v>5</v>
       </c>
       <c r="R17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -1919,19 +1908,19 @@
         <v>0</v>
       </c>
       <c r="O18" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P18" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q18">
         <v>5</v>
       </c>
       <c r="R18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" hidden="1">
       <c r="A19">
         <v>200</v>
       </c>
@@ -1984,7 +1973,7 @@
         <v>3</v>
       </c>
       <c r="R19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -2031,16 +2020,16 @@
         <v>0</v>
       </c>
       <c r="O20" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P20" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q20">
         <v>4</v>
       </c>
       <c r="R20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:18">
@@ -2087,16 +2076,16 @@
         <v>0</v>
       </c>
       <c r="O21" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P21" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="Q21">
         <v>1</v>
       </c>
       <c r="R21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:18">
@@ -2143,16 +2132,16 @@
         <v>0</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="Q22" s="1">
         <v>3</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:18">
@@ -2199,16 +2188,16 @@
         <v>0</v>
       </c>
       <c r="O23" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P23" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="Q23">
         <v>3</v>
       </c>
       <c r="R23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:18">
@@ -2255,19 +2244,19 @@
         <v>0</v>
       </c>
       <c r="O24" t="s">
-        <v>24</v>
+        <v>150</v>
       </c>
       <c r="P24" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
       <c r="Q24">
         <v>1</v>
       </c>
       <c r="R24" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" hidden="1">
       <c r="A25">
         <v>206</v>
       </c>
@@ -2320,7 +2309,7 @@
         <v>1</v>
       </c>
       <c r="R25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:18">
@@ -2367,16 +2356,16 @@
         <v>0</v>
       </c>
       <c r="O26" t="s">
-        <v>47</v>
+        <v>148</v>
       </c>
       <c r="P26" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q26">
         <v>2</v>
       </c>
       <c r="R26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:18">
@@ -2423,16 +2412,16 @@
         <v>0</v>
       </c>
       <c r="O27" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P27" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
       <c r="Q27">
         <v>1</v>
       </c>
       <c r="R27" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:18">
@@ -2479,16 +2468,16 @@
         <v>0</v>
       </c>
       <c r="O28" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="P28" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="Q28">
         <v>4</v>
       </c>
       <c r="R28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:18">
@@ -2535,16 +2524,16 @@
         <v>0</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>24</v>
+        <v>150</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q29" s="1">
         <v>4</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:18">
@@ -2591,16 +2580,16 @@
         <v>0</v>
       </c>
       <c r="O30" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P30" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q30">
         <v>2</v>
       </c>
       <c r="R30" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:18">
@@ -2647,19 +2636,19 @@
         <v>0</v>
       </c>
       <c r="O31" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P31" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="Q31">
         <v>4</v>
       </c>
       <c r="R31" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" hidden="1">
       <c r="A32">
         <v>213</v>
       </c>
@@ -2712,7 +2701,7 @@
         <v>4</v>
       </c>
       <c r="R32" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:18">
@@ -2759,19 +2748,19 @@
         <v>0</v>
       </c>
       <c r="O33" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P33" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q33">
         <v>3</v>
       </c>
       <c r="R33" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" hidden="1">
       <c r="A34">
         <v>215</v>
       </c>
@@ -2824,7 +2813,7 @@
         <v>2</v>
       </c>
       <c r="R34" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:18">
@@ -2871,16 +2860,16 @@
         <v>0</v>
       </c>
       <c r="O35" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P35" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q35">
         <v>4</v>
       </c>
       <c r="R35" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:18">
@@ -2927,16 +2916,16 @@
         <v>0</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q36" s="1">
         <v>3</v>
       </c>
       <c r="R36" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:18">
@@ -2983,16 +2972,16 @@
         <v>0</v>
       </c>
       <c r="O37" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P37" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="Q37">
         <v>2</v>
       </c>
       <c r="R37" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:18">
@@ -3039,16 +3028,16 @@
         <v>0</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>24</v>
+        <v>150</v>
       </c>
       <c r="Q38" s="1">
         <v>4</v>
       </c>
       <c r="R38" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:18">
@@ -3095,16 +3084,16 @@
         <v>0</v>
       </c>
       <c r="O39" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P39" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="Q39">
         <v>1</v>
       </c>
       <c r="R39" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:18">
@@ -3151,19 +3140,19 @@
         <v>0</v>
       </c>
       <c r="O40" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P40" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q40">
         <v>1</v>
       </c>
       <c r="R40" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" hidden="1">
       <c r="A41">
         <v>223</v>
       </c>
@@ -3216,7 +3205,7 @@
         <v>1</v>
       </c>
       <c r="R41" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:18">
@@ -3263,19 +3252,19 @@
         <v>0</v>
       </c>
       <c r="O42" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="P42" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
       <c r="Q42">
         <v>2</v>
       </c>
       <c r="R42" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" hidden="1">
       <c r="A43">
         <v>225</v>
       </c>
@@ -3328,10 +3317,10 @@
         <v>3</v>
       </c>
       <c r="R43" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" hidden="1">
       <c r="A44">
         <v>226</v>
       </c>
@@ -3384,10 +3373,10 @@
         <v>2</v>
       </c>
       <c r="R44" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" hidden="1">
       <c r="A45">
         <v>227</v>
       </c>
@@ -3440,7 +3429,7 @@
         <v>4</v>
       </c>
       <c r="R45" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:18">
@@ -3453,11 +3442,11 @@
       <c r="C46" s="2">
         <v>1</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>68</v>
+      <c r="D46" s="2">
+        <v>0</v>
+      </c>
+      <c r="E46" s="2">
+        <v>0</v>
       </c>
       <c r="F46" s="2">
         <v>0</v>
@@ -3487,16 +3476,16 @@
         <v>0</v>
       </c>
       <c r="O46" s="2" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P46" s="2" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q46" s="2">
         <v>2</v>
       </c>
       <c r="R46" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="1:18">
@@ -3543,16 +3532,16 @@
         <v>0</v>
       </c>
       <c r="O47" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="P47" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="Q47">
         <v>4</v>
       </c>
       <c r="R47" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:18">
@@ -3599,16 +3588,16 @@
         <v>0</v>
       </c>
       <c r="O48" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="P48" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q48">
         <v>3</v>
       </c>
       <c r="R48" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" spans="1:18">
@@ -3655,16 +3644,16 @@
         <v>1</v>
       </c>
       <c r="O49" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P49" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q49">
         <v>3</v>
       </c>
       <c r="R49" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:18">
@@ -3686,11 +3675,11 @@
       <c r="F50" s="2">
         <v>0</v>
       </c>
-      <c r="G50" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>73</v>
+      <c r="G50" s="2">
+        <v>0</v>
+      </c>
+      <c r="H50" s="2">
+        <v>0</v>
       </c>
       <c r="I50" s="2">
         <v>0</v>
@@ -3698,29 +3687,29 @@
       <c r="J50" s="2">
         <v>0</v>
       </c>
-      <c r="K50" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="L50" s="2" t="s">
-        <v>73</v>
+      <c r="K50" s="2">
+        <v>0</v>
+      </c>
+      <c r="L50" s="2">
+        <v>0</v>
       </c>
       <c r="M50" s="2">
         <v>1</v>
       </c>
-      <c r="N50" s="2" t="s">
-        <v>75</v>
+      <c r="N50" s="2">
+        <v>0</v>
       </c>
       <c r="O50" s="2" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P50" s="2" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q50" s="2">
         <v>3</v>
       </c>
       <c r="R50" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="51" spans="1:18">
@@ -3767,16 +3756,16 @@
         <v>0</v>
       </c>
       <c r="O51" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P51" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q51">
         <v>2</v>
       </c>
       <c r="R51" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:18">
@@ -3823,19 +3812,19 @@
         <v>0</v>
       </c>
       <c r="O52" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P52" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="Q52">
         <v>3</v>
       </c>
       <c r="R52" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="53" spans="1:18">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" hidden="1">
       <c r="A53">
         <v>235</v>
       </c>
@@ -3888,10 +3877,10 @@
         <v>2</v>
       </c>
       <c r="R53" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" hidden="1">
       <c r="A54">
         <v>236</v>
       </c>
@@ -3944,7 +3933,7 @@
         <v>3</v>
       </c>
       <c r="R54" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:18">
@@ -3991,16 +3980,16 @@
         <v>0</v>
       </c>
       <c r="O55" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P55" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q55">
         <v>2</v>
       </c>
       <c r="R55" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="56" spans="1:18">
@@ -4047,19 +4036,19 @@
         <v>0</v>
       </c>
       <c r="O56" s="1" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P56" s="1" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="Q56" s="1">
         <v>1</v>
       </c>
       <c r="R56" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" hidden="1">
       <c r="A57" s="1">
         <v>239</v>
       </c>
@@ -4112,7 +4101,7 @@
         <v>5</v>
       </c>
       <c r="R57" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="58" spans="1:18">
@@ -4159,16 +4148,16 @@
         <v>0</v>
       </c>
       <c r="O58" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P58" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q58">
         <v>3</v>
       </c>
       <c r="R58" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="59" spans="1:18">
@@ -4215,16 +4204,16 @@
         <v>0</v>
       </c>
       <c r="O59" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P59" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q59">
         <v>4</v>
       </c>
       <c r="R59" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="60" spans="1:18">
@@ -4271,16 +4260,16 @@
         <v>0</v>
       </c>
       <c r="O60" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P60" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
       <c r="Q60">
         <v>1</v>
       </c>
       <c r="R60" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="61" spans="1:18">
@@ -4327,19 +4316,19 @@
         <v>0</v>
       </c>
       <c r="O61" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P61" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="Q61">
         <v>2</v>
       </c>
       <c r="R61" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="62" spans="1:18">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" hidden="1">
       <c r="A62" s="1">
         <v>244</v>
       </c>
@@ -4392,10 +4381,10 @@
         <v>3</v>
       </c>
       <c r="R62" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="63" spans="1:18">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" hidden="1">
       <c r="A63">
         <v>245</v>
       </c>
@@ -4448,7 +4437,7 @@
         <v>3</v>
       </c>
       <c r="R63" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="64" spans="1:18">
@@ -4495,19 +4484,19 @@
         <v>0</v>
       </c>
       <c r="O64" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P64" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q64">
         <v>5</v>
       </c>
       <c r="R64" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" hidden="1">
       <c r="A65">
         <v>247</v>
       </c>
@@ -4560,7 +4549,7 @@
         <v>2</v>
       </c>
       <c r="R65" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="66" spans="1:18">
@@ -4607,16 +4596,16 @@
         <v>0</v>
       </c>
       <c r="O66" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P66" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q66">
         <v>2</v>
       </c>
       <c r="R66" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="67" spans="1:18">
@@ -4663,16 +4652,16 @@
         <v>1</v>
       </c>
       <c r="O67" s="1" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="P67" s="1" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="Q67" s="1">
         <v>3</v>
       </c>
       <c r="R67" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="68" spans="1:18">
@@ -4719,16 +4708,16 @@
         <v>0</v>
       </c>
       <c r="O68" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P68" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q68">
         <v>4</v>
       </c>
       <c r="R68" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
     </row>
     <row r="69" spans="1:18">
@@ -4775,16 +4764,16 @@
         <v>0</v>
       </c>
       <c r="O69" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P69" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q69">
         <v>3</v>
       </c>
       <c r="R69" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
     </row>
     <row r="70" spans="1:18">
@@ -4831,16 +4820,16 @@
         <v>0</v>
       </c>
       <c r="O70" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P70" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q70">
         <v>1</v>
       </c>
       <c r="R70" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="71" spans="1:18">
@@ -4887,16 +4876,16 @@
         <v>0</v>
       </c>
       <c r="O71" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="P71" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q71">
         <v>4</v>
       </c>
       <c r="R71" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="72" spans="1:18">
@@ -4943,16 +4932,16 @@
         <v>0</v>
       </c>
       <c r="O72" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P72" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
       <c r="Q72">
         <v>4</v>
       </c>
       <c r="R72" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="73" spans="1:18">
@@ -4999,19 +4988,19 @@
         <v>0</v>
       </c>
       <c r="O73" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="P73" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q73">
         <v>1</v>
       </c>
       <c r="R73" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="74" spans="1:18">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" hidden="1">
       <c r="A74">
         <v>256</v>
       </c>
@@ -5064,10 +5053,10 @@
         <v>4</v>
       </c>
       <c r="R74" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="75" spans="1:18">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" hidden="1">
       <c r="A75">
         <v>257</v>
       </c>
@@ -5120,7 +5109,7 @@
         <v>2</v>
       </c>
       <c r="R75" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="76" spans="1:18">
@@ -5167,19 +5156,19 @@
         <v>0</v>
       </c>
       <c r="O76" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P76" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q76">
         <v>2</v>
       </c>
       <c r="R76" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="77" spans="1:18">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" hidden="1">
       <c r="A77">
         <v>259</v>
       </c>
@@ -5232,7 +5221,7 @@
         <v>2</v>
       </c>
       <c r="R77" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="78" spans="1:18">
@@ -5279,19 +5268,19 @@
         <v>0</v>
       </c>
       <c r="O78" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P78" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q78">
         <v>2</v>
       </c>
       <c r="R78" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="79" spans="1:18">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" hidden="1">
       <c r="A79">
         <v>261</v>
       </c>
@@ -5344,7 +5333,7 @@
         <v>4</v>
       </c>
       <c r="R79" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="80" spans="1:18">
@@ -5391,16 +5380,16 @@
         <v>0</v>
       </c>
       <c r="O80" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P80" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q80">
         <v>2</v>
       </c>
       <c r="R80" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="81" spans="1:18">
@@ -5447,16 +5436,16 @@
         <v>0</v>
       </c>
       <c r="O81" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P81" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q81">
         <v>2</v>
       </c>
       <c r="R81" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="82" spans="1:18">
@@ -5503,16 +5492,16 @@
         <v>0</v>
       </c>
       <c r="O82" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P82" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="Q82">
         <v>2</v>
       </c>
       <c r="R82" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="83" spans="1:18">
@@ -5559,16 +5548,16 @@
         <v>0</v>
       </c>
       <c r="O83" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P83" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q83">
         <v>4</v>
       </c>
       <c r="R83" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="84" spans="1:18">
@@ -5615,16 +5604,16 @@
         <v>0</v>
       </c>
       <c r="O84" s="1" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="P84" s="1" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="Q84" s="1">
         <v>1</v>
       </c>
       <c r="R84" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="85" spans="1:18">
@@ -5671,16 +5660,16 @@
         <v>1</v>
       </c>
       <c r="O85" s="1" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P85" s="1" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q85" s="1">
         <v>4</v>
       </c>
       <c r="R85" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="86" spans="1:18">
@@ -5727,16 +5716,16 @@
         <v>1</v>
       </c>
       <c r="O86" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P86" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="Q86">
         <v>2</v>
       </c>
       <c r="R86" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="87" spans="1:18">
@@ -5783,19 +5772,19 @@
         <v>0</v>
       </c>
       <c r="O87" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P87" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q87">
         <v>2</v>
       </c>
       <c r="R87" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="88" spans="1:18">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" hidden="1">
       <c r="A88">
         <v>270</v>
       </c>
@@ -5848,7 +5837,7 @@
         <v>2</v>
       </c>
       <c r="R88" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="89" spans="1:18">
@@ -5895,19 +5884,19 @@
         <v>0</v>
       </c>
       <c r="O89" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="P89" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q89">
         <v>4</v>
       </c>
       <c r="R89" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="90" spans="1:18">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" hidden="1">
       <c r="A90">
         <v>272</v>
       </c>
@@ -5960,10 +5949,10 @@
         <v>2</v>
       </c>
       <c r="R90" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="91" spans="1:18">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" hidden="1">
       <c r="A91">
         <v>273</v>
       </c>
@@ -6016,7 +6005,7 @@
         <v>2</v>
       </c>
       <c r="R91" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="92" spans="1:18">
@@ -6063,16 +6052,16 @@
         <v>0</v>
       </c>
       <c r="O92" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P92" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="Q92">
         <v>4</v>
       </c>
       <c r="R92" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="93" spans="1:18">
@@ -6119,16 +6108,16 @@
         <v>0</v>
       </c>
       <c r="O93" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P93" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
       <c r="Q93">
         <v>2</v>
       </c>
       <c r="R93" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="94" spans="1:18">
@@ -6175,16 +6164,16 @@
         <v>0</v>
       </c>
       <c r="O94" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P94" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="Q94">
         <v>2</v>
       </c>
       <c r="R94" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="95" spans="1:18">
@@ -6231,16 +6220,16 @@
         <v>0</v>
       </c>
       <c r="O95" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P95" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="Q95">
         <v>2</v>
       </c>
       <c r="R95" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="96" spans="1:18">
@@ -6287,19 +6276,19 @@
         <v>0</v>
       </c>
       <c r="O96" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P96" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
       <c r="Q96">
         <v>2</v>
       </c>
       <c r="R96" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="97" spans="1:18">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" hidden="1">
       <c r="A97">
         <v>279</v>
       </c>
@@ -6352,7 +6341,7 @@
         <v>2</v>
       </c>
       <c r="R97" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="98" spans="1:18">
@@ -6399,16 +6388,16 @@
         <v>0</v>
       </c>
       <c r="O98" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P98" t="s">
-        <v>121</v>
+        <v>151</v>
       </c>
       <c r="Q98">
         <v>2</v>
       </c>
       <c r="R98" s="3" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="99" spans="1:18">
@@ -6455,16 +6444,16 @@
         <v>1</v>
       </c>
       <c r="O99" s="1" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="P99" s="1" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="Q99" s="1">
         <v>5</v>
       </c>
       <c r="R99" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="100" spans="1:18">
@@ -6511,16 +6500,16 @@
         <v>0</v>
       </c>
       <c r="O100" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P100" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q100">
         <v>3</v>
       </c>
       <c r="R100" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="101" spans="1:18">
@@ -6567,19 +6556,19 @@
         <v>0</v>
       </c>
       <c r="O101" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P101" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="Q101">
         <v>1</v>
       </c>
       <c r="R101" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="102" spans="1:18">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" hidden="1">
       <c r="A102" s="1">
         <v>285</v>
       </c>
@@ -6632,7 +6621,7 @@
         <v>1</v>
       </c>
       <c r="R102" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="103" spans="1:18">
@@ -6679,16 +6668,16 @@
         <v>0</v>
       </c>
       <c r="O103" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P103" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q103">
         <v>4</v>
       </c>
       <c r="R103" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="104" spans="1:18">
@@ -6735,16 +6724,16 @@
         <v>0</v>
       </c>
       <c r="O104" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P104" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q104">
         <v>2</v>
       </c>
       <c r="R104" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="105" spans="1:18">
@@ -6791,19 +6780,19 @@
         <v>0</v>
       </c>
       <c r="O105" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P105" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q105">
         <v>1</v>
       </c>
       <c r="R105" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="106" spans="1:18">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" hidden="1">
       <c r="A106" s="2">
         <v>289</v>
       </c>
@@ -6846,17 +6835,13 @@
       <c r="N106" s="2">
         <v>0</v>
       </c>
-      <c r="O106" s="2" t="s">
-        <v>131</v>
-      </c>
+      <c r="O106" s="2"/>
       <c r="P106" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="Q106" s="2" t="s">
-        <v>132</v>
-      </c>
+      <c r="Q106" s="2"/>
       <c r="R106" s="2" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="107" spans="1:18">
@@ -6903,16 +6888,16 @@
         <v>0</v>
       </c>
       <c r="O107" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="P107" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q107">
         <v>4</v>
       </c>
       <c r="R107" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
     <row r="108" spans="1:18">
@@ -6959,19 +6944,19 @@
         <v>0</v>
       </c>
       <c r="O108" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P108" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
       <c r="Q108">
         <v>4</v>
       </c>
       <c r="R108" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="109" spans="1:18">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="109" spans="1:18" hidden="1">
       <c r="A109">
         <v>292</v>
       </c>
@@ -7024,7 +7009,7 @@
         <v>2</v>
       </c>
       <c r="R109" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
     <row r="110" spans="1:18">
@@ -7071,16 +7056,16 @@
         <v>0</v>
       </c>
       <c r="O110" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P110" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="Q110">
         <v>1</v>
       </c>
       <c r="R110" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="111" spans="1:18">
@@ -7127,16 +7112,16 @@
         <v>1</v>
       </c>
       <c r="O111" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P111" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q111">
         <v>5</v>
       </c>
       <c r="R111" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="112" spans="1:18">
@@ -7183,16 +7168,16 @@
         <v>0</v>
       </c>
       <c r="O112" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P112" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q112">
         <v>4</v>
       </c>
       <c r="R112" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
     </row>
     <row r="113" spans="1:18">
@@ -7239,16 +7224,16 @@
         <v>0</v>
       </c>
       <c r="O113" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P113" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q113">
         <v>1</v>
       </c>
       <c r="R113" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
     </row>
     <row r="114" spans="1:18">
@@ -7295,19 +7280,19 @@
         <v>0</v>
       </c>
       <c r="O114" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P114" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q114">
         <v>4</v>
       </c>
       <c r="R114" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="115" spans="1:18">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="115" spans="1:18" hidden="1">
       <c r="A115">
         <v>298</v>
       </c>
@@ -7360,7 +7345,7 @@
         <v>2</v>
       </c>
       <c r="R115" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="116" spans="1:18">
@@ -7407,16 +7392,16 @@
         <v>0</v>
       </c>
       <c r="O116" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P116" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q116">
         <v>1</v>
       </c>
       <c r="R116" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
     </row>
     <row r="117" spans="1:18">
@@ -7453,8 +7438,8 @@
       <c r="K117">
         <v>0</v>
       </c>
-      <c r="L117" t="s">
-        <v>144</v>
+      <c r="L117">
+        <v>1</v>
       </c>
       <c r="M117">
         <v>0</v>
@@ -7463,16 +7448,16 @@
         <v>0</v>
       </c>
       <c r="O117" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P117" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
       <c r="Q117">
         <v>4</v>
       </c>
       <c r="R117" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="118" spans="1:18">
@@ -7519,16 +7504,16 @@
         <v>0</v>
       </c>
       <c r="O118" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="P118" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q118">
         <v>4</v>
       </c>
       <c r="R118" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="119" spans="1:18">
@@ -7575,16 +7560,16 @@
         <v>0</v>
       </c>
       <c r="O119" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P119" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q119">
         <v>3</v>
       </c>
       <c r="R119" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="120" spans="1:18">
@@ -7631,16 +7616,16 @@
         <v>0</v>
       </c>
       <c r="O120" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P120" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q120">
         <v>4</v>
       </c>
       <c r="R120" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="121" spans="1:18">
@@ -7687,19 +7672,19 @@
         <v>0</v>
       </c>
       <c r="O121" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P121" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q121">
         <v>2</v>
       </c>
       <c r="R121" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="122" spans="1:18">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="122" spans="1:18" hidden="1">
       <c r="A122">
         <v>305</v>
       </c>
@@ -7752,7 +7737,7 @@
         <v>3</v>
       </c>
       <c r="R122" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="123" spans="1:18">
@@ -7799,19 +7784,19 @@
         <v>0</v>
       </c>
       <c r="O123" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P123" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q123">
         <v>5</v>
       </c>
       <c r="R123" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="124" spans="1:18">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="124" spans="1:18" hidden="1">
       <c r="A124">
         <v>307</v>
       </c>
@@ -7864,7 +7849,7 @@
         <v>2</v>
       </c>
       <c r="R124" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
     </row>
     <row r="125" spans="1:18">
@@ -7911,19 +7896,27 @@
         <v>0</v>
       </c>
       <c r="O125" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="P125" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="Q125">
         <v>3</v>
       </c>
       <c r="R125" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:R125">
+    <filterColumn colId="14">
+      <filters>
+        <filter val="no"/>
+        <filter val="yes"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Removed superfluous columns from Debrief_TG.xlsx.
</commit_message>
<xml_diff>
--- a/raw-data-prep/raw_data/Debrief_TG.xlsx
+++ b/raw-data-prep/raw_data/Debrief_TG.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8235"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="229">
   <si>
     <t>Subject</t>
   </si>
@@ -151,15 +151,6 @@
   </si>
   <si>
     <t>Maybe just ask.</t>
-  </si>
-  <si>
-    <t>Note: Condition 3</t>
-  </si>
-  <si>
-    <t>Note: Condition 2</t>
-  </si>
-  <si>
-    <t>Note: Condtition 2</t>
   </si>
   <si>
     <t>To see how much  we would hate each other?</t>
@@ -212,9 +203,6 @@
     <t>I think it was based of how we felt about our partners eveluation</t>
   </si>
   <si>
-    <t xml:space="preserve">Note: Condition 2 </t>
-  </si>
-  <si>
     <t>So you could see how their evaluation of our essay affecteed us</t>
   </si>
   <si>
@@ -233,18 +221,12 @@
     <t>Most likely if we were angered at the other participanta judging of our essays, we would give a stringer distraction</t>
   </si>
   <si>
-    <t>Note :Condition 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">To see if the other persons response made us mad if it did we would assign them a large distraction. </t>
   </si>
   <si>
     <t>to test aggression/anger from the evaluated essay</t>
   </si>
   <si>
-    <t>Note: condition 4</t>
-  </si>
-  <si>
     <t>to get back at the other person if they evaluated your essay on the other topic</t>
   </si>
   <si>
@@ -311,9 +293,6 @@
     <t xml:space="preserve">Agression towards other participants critisism. </t>
   </si>
   <si>
-    <t xml:space="preserve">Note: Condition 3 </t>
-  </si>
-  <si>
     <t>To see if the score our partner gave us would make us angry and give them a longer distraction time</t>
   </si>
   <si>
@@ -329,9 +308,6 @@
     <t xml:space="preserve">to see how we would punish someone with differing views on a controversial topic </t>
   </si>
   <si>
-    <t>note: square next to number</t>
-  </si>
-  <si>
     <t>To see how we would respond to our essay evaluations</t>
   </si>
   <si>
@@ -347,9 +323,6 @@
     <t>To see if how we punished are partners based off their evaluation</t>
   </si>
   <si>
-    <t xml:space="preserve">note: condition 1 </t>
-  </si>
-  <si>
     <t>To eliminate fear or any sort of bias that may exist</t>
   </si>
   <si>
@@ -395,13 +368,7 @@
     <t xml:space="preserve">TO SEE HOW AGGRESSIVE WE FELT AFTER PLAYING AN AGGRESSIVE VIDEO GAME </t>
   </si>
   <si>
-    <t>note: condition 2</t>
-  </si>
-  <si>
     <t>To see how mad I was at the way he judged my paper.</t>
-  </si>
-  <si>
-    <t>note: condition 3</t>
   </si>
   <si>
     <t>To have a more random variable</t>
@@ -464,9 +431,6 @@
     <t>Because the video game may make me aggressive., so I may choose the longest time. But actually, the comments makes me feel not good very nuch</t>
   </si>
   <si>
-    <t>Note: condition 2</t>
-  </si>
-  <si>
     <t>To show how agrivated we get against the other person for their response on my essay.</t>
   </si>
   <si>
@@ -474,9 +438,6 @@
   </si>
   <si>
     <t>To see if we were against our partner after seeing their response to the essay</t>
-  </si>
-  <si>
-    <t>note: condition 1</t>
   </si>
   <si>
     <t>Since they showed us our partners response that was negitive, it would see if we wanted to be more agressice to the other person.</t>
@@ -878,6 +839,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -925,7 +889,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -960,7 +924,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1169,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI197"/>
+  <dimension ref="A1:R197"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O131" sqref="O131"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:AA1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1180,7 +1144,7 @@
     <col min="15" max="15" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1236,7 +1200,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>183</v>
       </c>
@@ -1292,7 +1256,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>184</v>
       </c>
@@ -1348,7 +1312,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>185</v>
       </c>
@@ -1404,7 +1368,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>168</v>
       </c>
@@ -1459,21 +1423,8 @@
       <c r="R5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-      <c r="AC5" s="1"/>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>187</v>
       </c>
@@ -1529,7 +1480,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>189</v>
       </c>
@@ -1585,7 +1536,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>188</v>
       </c>
@@ -1641,7 +1592,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>190</v>
       </c>
@@ -1697,7 +1648,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>191</v>
       </c>
@@ -1753,7 +1704,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>192</v>
       </c>
@@ -1809,7 +1760,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>193</v>
       </c>
@@ -1865,7 +1816,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>194</v>
       </c>
@@ -1920,21 +1871,8 @@
       <c r="R13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
-      <c r="V13" s="1"/>
-      <c r="W13" s="1"/>
-      <c r="X13" s="1"/>
-      <c r="Y13" s="1"/>
-      <c r="Z13" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA13" s="1"/>
-      <c r="AB13" s="1"/>
-      <c r="AC13" s="1"/>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>195</v>
       </c>
@@ -1990,7 +1928,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>196</v>
       </c>
@@ -2046,7 +1984,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>197</v>
       </c>
@@ -2102,7 +2040,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>199</v>
       </c>
@@ -2158,7 +2096,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>198</v>
       </c>
@@ -2214,7 +2152,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>200</v>
       </c>
@@ -2270,7 +2208,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>201</v>
       </c>
@@ -2326,7 +2264,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>202</v>
       </c>
@@ -2382,7 +2320,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>203</v>
       </c>
@@ -2437,21 +2375,8 @@
       <c r="R22" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S22" s="1"/>
-      <c r="T22" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="U22" s="1"/>
-      <c r="V22" s="1"/>
-      <c r="W22" s="1"/>
-      <c r="X22" s="1"/>
-      <c r="Y22" s="1"/>
-      <c r="Z22" s="1"/>
-      <c r="AA22" s="1"/>
-      <c r="AB22" s="1"/>
-      <c r="AC22" s="1"/>
-    </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>204</v>
       </c>
@@ -2504,10 +2429,10 @@
         <v>3</v>
       </c>
       <c r="R23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>205</v>
       </c>
@@ -2560,10 +2485,10 @@
         <v>1</v>
       </c>
       <c r="R24" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>206</v>
       </c>
@@ -2616,10 +2541,10 @@
         <v>1</v>
       </c>
       <c r="R25" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>207</v>
       </c>
@@ -2663,7 +2588,7 @@
         <v>0</v>
       </c>
       <c r="O26" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="P26" t="s">
         <v>19</v>
@@ -2672,10 +2597,10 @@
         <v>2</v>
       </c>
       <c r="R26" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>208</v>
       </c>
@@ -2728,10 +2653,10 @@
         <v>1</v>
       </c>
       <c r="R27" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>209</v>
       </c>
@@ -2784,10 +2709,10 @@
         <v>4</v>
       </c>
       <c r="R28" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>210</v>
       </c>
@@ -2840,23 +2765,10 @@
         <v>4</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="S29" s="1"/>
-      <c r="T29" s="1"/>
-      <c r="U29" s="1"/>
-      <c r="V29" s="1"/>
-      <c r="W29" s="1"/>
-      <c r="X29" s="1"/>
-      <c r="Y29" s="1"/>
-      <c r="Z29" s="1"/>
-      <c r="AA29" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB29" s="1"/>
-      <c r="AC29" s="1"/>
-    </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>211</v>
       </c>
@@ -2909,10 +2821,10 @@
         <v>2</v>
       </c>
       <c r="R30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>212</v>
       </c>
@@ -2965,10 +2877,10 @@
         <v>4</v>
       </c>
       <c r="R31" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>213</v>
       </c>
@@ -3021,10 +2933,10 @@
         <v>4</v>
       </c>
       <c r="R32" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>214</v>
       </c>
@@ -3077,10 +2989,10 @@
         <v>3</v>
       </c>
       <c r="R33" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>215</v>
       </c>
@@ -3133,10 +3045,10 @@
         <v>2</v>
       </c>
       <c r="R34" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>217</v>
       </c>
@@ -3189,10 +3101,10 @@
         <v>4</v>
       </c>
       <c r="R35" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>218</v>
       </c>
@@ -3245,24 +3157,10 @@
         <v>3</v>
       </c>
       <c r="R36" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="S36" s="1"/>
-      <c r="T36" s="1"/>
-      <c r="U36" s="1"/>
-      <c r="V36" s="1"/>
-      <c r="W36" s="1"/>
-      <c r="X36" s="1"/>
-      <c r="Y36" s="1"/>
-      <c r="Z36" s="1"/>
-      <c r="AA36" s="1"/>
-      <c r="AB36" s="1"/>
-      <c r="AC36" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="AD36" s="1"/>
-    </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>219</v>
       </c>
@@ -3315,10 +3213,10 @@
         <v>2</v>
       </c>
       <c r="R37" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>220</v>
       </c>
@@ -3371,24 +3269,10 @@
         <v>4</v>
       </c>
       <c r="R38" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="S38" s="1"/>
-      <c r="T38" s="1"/>
-      <c r="U38" s="1"/>
-      <c r="V38" s="1"/>
-      <c r="W38" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="X38" s="1"/>
-      <c r="Y38" s="1"/>
-      <c r="Z38" s="1"/>
-      <c r="AA38" s="1"/>
-      <c r="AB38" s="1"/>
-      <c r="AC38" s="1"/>
-      <c r="AD38" s="1"/>
-    </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>221</v>
       </c>
@@ -3441,10 +3325,10 @@
         <v>1</v>
       </c>
       <c r="R39" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>222</v>
       </c>
@@ -3497,10 +3381,10 @@
         <v>1</v>
       </c>
       <c r="R40" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>223</v>
       </c>
@@ -3553,10 +3437,10 @@
         <v>1</v>
       </c>
       <c r="R41" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>224</v>
       </c>
@@ -3609,10 +3493,10 @@
         <v>2</v>
       </c>
       <c r="R42" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>225</v>
       </c>
@@ -3665,10 +3549,10 @@
         <v>3</v>
       </c>
       <c r="R43" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>226</v>
       </c>
@@ -3721,10 +3605,10 @@
         <v>2</v>
       </c>
       <c r="R44" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>227</v>
       </c>
@@ -3777,10 +3661,10 @@
         <v>4</v>
       </c>
       <c r="R45" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>228</v>
       </c>
@@ -3791,10 +3675,10 @@
         <v>1</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F46" s="2">
         <v>0</v>
@@ -3833,21 +3717,10 @@
         <v>2</v>
       </c>
       <c r="R46" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="S46" s="2"/>
-      <c r="T46" s="2"/>
-      <c r="U46" s="2"/>
-      <c r="V46" s="2"/>
-      <c r="W46" s="2"/>
-      <c r="X46" s="2"/>
-      <c r="Y46" s="2"/>
-      <c r="Z46" s="2"/>
-      <c r="AA46" s="2"/>
-      <c r="AB46" s="2"/>
-      <c r="AC46" s="2"/>
-    </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>229</v>
       </c>
@@ -3900,10 +3773,10 @@
         <v>4</v>
       </c>
       <c r="R47" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>230</v>
       </c>
@@ -3956,10 +3829,10 @@
         <v>3</v>
       </c>
       <c r="R48" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>231</v>
       </c>
@@ -4012,10 +3885,10 @@
         <v>3</v>
       </c>
       <c r="R49" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>232</v>
       </c>
@@ -4035,10 +3908,10 @@
         <v>0</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="I50" s="2">
         <v>0</v>
@@ -4047,16 +3920,16 @@
         <v>0</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="M50" s="2">
         <v>1</v>
       </c>
       <c r="N50" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="O50" s="2" t="s">
         <v>19</v>
@@ -4068,21 +3941,10 @@
         <v>3</v>
       </c>
       <c r="R50" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="S50" s="2"/>
-      <c r="T50" s="2"/>
-      <c r="U50" s="2"/>
-      <c r="V50" s="2"/>
-      <c r="W50" s="2"/>
-      <c r="X50" s="2"/>
-      <c r="Y50" s="2"/>
-      <c r="Z50" s="2"/>
-      <c r="AA50" s="2"/>
-      <c r="AB50" s="2"/>
-      <c r="AC50" s="2"/>
-    </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>233</v>
       </c>
@@ -4135,10 +3997,10 @@
         <v>2</v>
       </c>
       <c r="R51" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>234</v>
       </c>
@@ -4191,10 +4053,10 @@
         <v>3</v>
       </c>
       <c r="R52" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>235</v>
       </c>
@@ -4247,10 +4109,10 @@
         <v>2</v>
       </c>
       <c r="R53" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>236</v>
       </c>
@@ -4303,10 +4165,10 @@
         <v>3</v>
       </c>
       <c r="R54" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>237</v>
       </c>
@@ -4359,10 +4221,10 @@
         <v>2</v>
       </c>
       <c r="R55" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>238</v>
       </c>
@@ -4415,25 +4277,10 @@
         <v>1</v>
       </c>
       <c r="R56" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="S56" s="1"/>
-      <c r="T56" s="1"/>
-      <c r="U56" s="1"/>
-      <c r="V56" s="1"/>
-      <c r="W56" s="1"/>
-      <c r="X56" s="1"/>
-      <c r="Y56" s="1"/>
-      <c r="Z56" s="1"/>
-      <c r="AA56" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB56" s="1"/>
-      <c r="AC56" s="1"/>
-      <c r="AD56" s="1"/>
-      <c r="AE56" s="1"/>
-    </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>239</v>
       </c>
@@ -4486,24 +4333,10 @@
         <v>5</v>
       </c>
       <c r="R57" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="S57" s="1"/>
-      <c r="T57" s="1"/>
-      <c r="U57" s="1"/>
-      <c r="V57" s="1"/>
-      <c r="W57" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="X57" s="1"/>
-      <c r="Y57" s="1"/>
-      <c r="Z57" s="1"/>
-      <c r="AA57" s="1"/>
-      <c r="AB57" s="1"/>
-      <c r="AC57" s="1"/>
-      <c r="AD57" s="1"/>
-    </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>240</v>
       </c>
@@ -4556,10 +4389,10 @@
         <v>3</v>
       </c>
       <c r="R58" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>241</v>
       </c>
@@ -4612,10 +4445,10 @@
         <v>4</v>
       </c>
       <c r="R59" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="60" spans="1:31" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>242</v>
       </c>
@@ -4668,10 +4501,10 @@
         <v>1</v>
       </c>
       <c r="R60" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>243</v>
       </c>
@@ -4724,10 +4557,10 @@
         <v>2</v>
       </c>
       <c r="R61" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="62" spans="1:31" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>244</v>
       </c>
@@ -4780,25 +4613,10 @@
         <v>3</v>
       </c>
       <c r="R62" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="S62" s="1"/>
-      <c r="T62" s="1"/>
-      <c r="U62" s="1"/>
-      <c r="V62" s="1"/>
-      <c r="W62" s="1"/>
-      <c r="X62" s="1"/>
-      <c r="Y62" s="1"/>
-      <c r="Z62" s="1"/>
-      <c r="AA62" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AB62" s="1"/>
-      <c r="AC62" s="1"/>
-      <c r="AD62" s="1"/>
-      <c r="AE62" s="1"/>
-    </row>
-    <row r="63" spans="1:31" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>245</v>
       </c>
@@ -4851,10 +4669,10 @@
         <v>3</v>
       </c>
       <c r="R63" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="64" spans="1:31" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>246</v>
       </c>
@@ -4907,10 +4725,10 @@
         <v>5</v>
       </c>
       <c r="R64" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="65" spans="1:31" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>247</v>
       </c>
@@ -4963,10 +4781,10 @@
         <v>2</v>
       </c>
       <c r="R65" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="66" spans="1:31" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>248</v>
       </c>
@@ -5019,10 +4837,10 @@
         <v>2</v>
       </c>
       <c r="R66" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="67" spans="1:31" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>249</v>
       </c>
@@ -5075,25 +4893,10 @@
         <v>3</v>
       </c>
       <c r="R67" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="S67" s="1"/>
-      <c r="T67" s="1"/>
-      <c r="U67" s="1"/>
-      <c r="V67" s="1"/>
-      <c r="W67" s="1"/>
-      <c r="X67" s="1"/>
-      <c r="Y67" s="1"/>
-      <c r="Z67" s="1"/>
-      <c r="AA67" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AB67" s="1"/>
-      <c r="AC67" s="1"/>
-      <c r="AD67" s="1"/>
-      <c r="AE67" s="1"/>
-    </row>
-    <row r="68" spans="1:31" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>250</v>
       </c>
@@ -5146,10 +4949,10 @@
         <v>4</v>
       </c>
       <c r="R68" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="69" spans="1:31" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>251</v>
       </c>
@@ -5202,10 +5005,10 @@
         <v>3</v>
       </c>
       <c r="R69" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="70" spans="1:31" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>252</v>
       </c>
@@ -5258,10 +5061,10 @@
         <v>1</v>
       </c>
       <c r="R70" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="71" spans="1:31" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>253</v>
       </c>
@@ -5314,10 +5117,10 @@
         <v>4</v>
       </c>
       <c r="R71" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="72" spans="1:31" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>254</v>
       </c>
@@ -5370,10 +5173,10 @@
         <v>4</v>
       </c>
       <c r="R72" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="73" spans="1:31" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>255</v>
       </c>
@@ -5426,10 +5229,10 @@
         <v>1</v>
       </c>
       <c r="R73" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="74" spans="1:31" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>256</v>
       </c>
@@ -5482,10 +5285,10 @@
         <v>4</v>
       </c>
       <c r="R74" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="75" spans="1:31" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>257</v>
       </c>
@@ -5538,10 +5341,10 @@
         <v>2</v>
       </c>
       <c r="R75" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="76" spans="1:31" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>258</v>
       </c>
@@ -5594,10 +5397,10 @@
         <v>2</v>
       </c>
       <c r="R76" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="77" spans="1:31" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>259</v>
       </c>
@@ -5650,10 +5453,10 @@
         <v>2</v>
       </c>
       <c r="R77" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="78" spans="1:31" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>260</v>
       </c>
@@ -5706,10 +5509,10 @@
         <v>2</v>
       </c>
       <c r="R78" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="79" spans="1:31" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>261</v>
       </c>
@@ -5762,10 +5565,10 @@
         <v>4</v>
       </c>
       <c r="R79" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="80" spans="1:31" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>262</v>
       </c>
@@ -5818,10 +5621,10 @@
         <v>2</v>
       </c>
       <c r="R80" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="81" spans="1:29" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>263</v>
       </c>
@@ -5874,10 +5677,10 @@
         <v>2</v>
       </c>
       <c r="R81" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="82" spans="1:29" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>264</v>
       </c>
@@ -5930,10 +5733,10 @@
         <v>2</v>
       </c>
       <c r="R82" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="83" spans="1:29" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>265</v>
       </c>
@@ -5986,10 +5789,10 @@
         <v>4</v>
       </c>
       <c r="R83" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="84" spans="1:29" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>266</v>
       </c>
@@ -6042,23 +5845,10 @@
         <v>1</v>
       </c>
       <c r="R84" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="S84" s="1"/>
-      <c r="T84" s="1"/>
-      <c r="U84" s="1"/>
-      <c r="V84" s="1"/>
-      <c r="W84" s="1"/>
-      <c r="X84" s="1"/>
-      <c r="Y84" s="1"/>
-      <c r="Z84" s="1"/>
-      <c r="AA84" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="AB84" s="1"/>
-      <c r="AC84" s="1"/>
-    </row>
-    <row r="85" spans="1:29" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>267</v>
       </c>
@@ -6111,23 +5901,10 @@
         <v>4</v>
       </c>
       <c r="R85" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="S85" s="1"/>
-      <c r="T85" s="1"/>
-      <c r="U85" s="1"/>
-      <c r="V85" s="1"/>
-      <c r="W85" s="1"/>
-      <c r="X85" s="1"/>
-      <c r="Y85" s="1"/>
-      <c r="Z85" s="1"/>
-      <c r="AA85" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="AB85" s="1"/>
-      <c r="AC85" s="1"/>
-    </row>
-    <row r="86" spans="1:29" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>268</v>
       </c>
@@ -6180,10 +5957,10 @@
         <v>2</v>
       </c>
       <c r="R86" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="87" spans="1:29" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>269</v>
       </c>
@@ -6236,10 +6013,10 @@
         <v>2</v>
       </c>
       <c r="R87" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="88" spans="1:29" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>270</v>
       </c>
@@ -6292,10 +6069,10 @@
         <v>2</v>
       </c>
       <c r="R88" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="89" spans="1:29" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>271</v>
       </c>
@@ -6348,10 +6125,10 @@
         <v>4</v>
       </c>
       <c r="R89" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="90" spans="1:29" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>272</v>
       </c>
@@ -6404,10 +6181,10 @@
         <v>2</v>
       </c>
       <c r="R90" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="91" spans="1:29" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>273</v>
       </c>
@@ -6460,10 +6237,10 @@
         <v>2</v>
       </c>
       <c r="R91" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="92" spans="1:29" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>274</v>
       </c>
@@ -6516,10 +6293,10 @@
         <v>4</v>
       </c>
       <c r="R92" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="93" spans="1:29" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>275</v>
       </c>
@@ -6572,10 +6349,10 @@
         <v>2</v>
       </c>
       <c r="R93" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="94" spans="1:29" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>276</v>
       </c>
@@ -6628,10 +6405,10 @@
         <v>2</v>
       </c>
       <c r="R94" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="95" spans="1:29" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>277</v>
       </c>
@@ -6684,10 +6461,10 @@
         <v>2</v>
       </c>
       <c r="R95" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="96" spans="1:29" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>278</v>
       </c>
@@ -6740,10 +6517,10 @@
         <v>2</v>
       </c>
       <c r="R96" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="97" spans="1:35" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>279</v>
       </c>
@@ -6796,10 +6573,10 @@
         <v>2</v>
       </c>
       <c r="R97" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="98" spans="1:35" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>281</v>
       </c>
@@ -6846,16 +6623,16 @@
         <v>19</v>
       </c>
       <c r="P98" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="Q98">
         <v>2</v>
       </c>
       <c r="R98" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="99" spans="1:35" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>282</v>
       </c>
@@ -6902,35 +6679,16 @@
         <v>18</v>
       </c>
       <c r="P99" s="1" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="Q99" s="1">
         <v>5</v>
       </c>
       <c r="R99" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="S99" s="1"/>
-      <c r="T99" s="1"/>
-      <c r="U99" s="1"/>
-      <c r="V99" s="1"/>
-      <c r="W99" s="1"/>
-      <c r="X99" s="1"/>
-      <c r="Y99" s="1"/>
-      <c r="Z99" s="1"/>
-      <c r="AA99" s="1"/>
-      <c r="AB99" s="1"/>
-      <c r="AC99" s="1"/>
-      <c r="AD99" s="1"/>
-      <c r="AE99" s="1"/>
-      <c r="AF99" s="1"/>
-      <c r="AG99" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="AH99" s="1"/>
-      <c r="AI99" s="1"/>
-    </row>
-    <row r="100" spans="1:35" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>283</v>
       </c>
@@ -6983,10 +6741,10 @@
         <v>3</v>
       </c>
       <c r="R100" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="101" spans="1:35" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>284</v>
       </c>
@@ -7039,10 +6797,10 @@
         <v>1</v>
       </c>
       <c r="R101" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="102" spans="1:35" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>285</v>
       </c>
@@ -7095,29 +6853,10 @@
         <v>1</v>
       </c>
       <c r="R102" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="S102" s="1"/>
-      <c r="T102" s="1"/>
-      <c r="U102" s="1"/>
-      <c r="V102" s="1"/>
-      <c r="W102" s="1"/>
-      <c r="X102" s="1"/>
-      <c r="Y102" s="1"/>
-      <c r="Z102" s="1"/>
-      <c r="AA102" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="AB102" s="1"/>
-      <c r="AC102" s="1"/>
-      <c r="AD102" s="1"/>
-      <c r="AE102" s="1"/>
-      <c r="AF102" s="1"/>
-      <c r="AG102" s="1"/>
-      <c r="AH102" s="1"/>
-      <c r="AI102" s="1"/>
-    </row>
-    <row r="103" spans="1:35" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>286</v>
       </c>
@@ -7170,10 +6909,10 @@
         <v>4</v>
       </c>
       <c r="R103" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="104" spans="1:35" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>287</v>
       </c>
@@ -7226,10 +6965,10 @@
         <v>2</v>
       </c>
       <c r="R104" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="105" spans="1:35" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>288</v>
       </c>
@@ -7282,10 +7021,10 @@
         <v>1</v>
       </c>
       <c r="R105" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="106" spans="1:35" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>289</v>
       </c>
@@ -7329,25 +7068,19 @@
         <v>0</v>
       </c>
       <c r="O106" s="2" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="P106" s="2" t="s">
         <v>19</v>
       </c>
       <c r="Q106" s="2" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="R106" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="S106" s="2"/>
-      <c r="T106" s="2"/>
-      <c r="U106" s="2"/>
-      <c r="V106" s="2"/>
-      <c r="W106" s="2"/>
-      <c r="X106" s="2"/>
-    </row>
-    <row r="107" spans="1:35" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>290</v>
       </c>
@@ -7400,10 +7133,10 @@
         <v>4</v>
       </c>
       <c r="R107" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="108" spans="1:35" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>291</v>
       </c>
@@ -7456,10 +7189,10 @@
         <v>4</v>
       </c>
       <c r="R108" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="109" spans="1:35" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>292</v>
       </c>
@@ -7512,10 +7245,10 @@
         <v>2</v>
       </c>
       <c r="R109" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="110" spans="1:35" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>293</v>
       </c>
@@ -7568,10 +7301,10 @@
         <v>1</v>
       </c>
       <c r="R110" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="111" spans="1:35" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>294</v>
       </c>
@@ -7624,10 +7357,10 @@
         <v>5</v>
       </c>
       <c r="R111" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="112" spans="1:35" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>295</v>
       </c>
@@ -7680,7 +7413,7 @@
         <v>4</v>
       </c>
       <c r="R112" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.25">
@@ -7736,7 +7469,7 @@
         <v>1</v>
       </c>
       <c r="R113" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
     </row>
     <row r="114" spans="1:18" x14ac:dyDescent="0.25">
@@ -7792,7 +7525,7 @@
         <v>4</v>
       </c>
       <c r="R114" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
     </row>
     <row r="115" spans="1:18" x14ac:dyDescent="0.25">
@@ -7848,7 +7581,7 @@
         <v>2</v>
       </c>
       <c r="R115" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.25">
@@ -7904,7 +7637,7 @@
         <v>1</v>
       </c>
       <c r="R116" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.25">
@@ -7942,7 +7675,7 @@
         <v>0</v>
       </c>
       <c r="L117" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="M117">
         <v>0</v>
@@ -7960,7 +7693,7 @@
         <v>4</v>
       </c>
       <c r="R117" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.25">
@@ -8016,7 +7749,7 @@
         <v>4</v>
       </c>
       <c r="R118" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.25">
@@ -8072,7 +7805,7 @@
         <v>3</v>
       </c>
       <c r="R119" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
     </row>
     <row r="120" spans="1:18" x14ac:dyDescent="0.25">
@@ -8128,7 +7861,7 @@
         <v>4</v>
       </c>
       <c r="R120" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
     </row>
     <row r="121" spans="1:18" x14ac:dyDescent="0.25">
@@ -8184,7 +7917,7 @@
         <v>2</v>
       </c>
       <c r="R121" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
     </row>
     <row r="122" spans="1:18" x14ac:dyDescent="0.25">
@@ -8240,7 +7973,7 @@
         <v>3</v>
       </c>
       <c r="R122" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
     </row>
     <row r="123" spans="1:18" x14ac:dyDescent="0.25">
@@ -8296,7 +8029,7 @@
         <v>5</v>
       </c>
       <c r="R123" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
     </row>
     <row r="124" spans="1:18" x14ac:dyDescent="0.25">
@@ -8352,7 +8085,7 @@
         <v>2</v>
       </c>
       <c r="R124" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
     </row>
     <row r="125" spans="1:18" x14ac:dyDescent="0.25">
@@ -8408,7 +8141,7 @@
         <v>3</v>
       </c>
       <c r="R125" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
     </row>
     <row r="126" spans="1:18" x14ac:dyDescent="0.25">
@@ -8464,7 +8197,7 @@
         <v>4</v>
       </c>
       <c r="R126" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
     </row>
     <row r="127" spans="1:18" x14ac:dyDescent="0.25">
@@ -8520,7 +8253,7 @@
         <v>4</v>
       </c>
       <c r="R127" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
     </row>
     <row r="128" spans="1:18" x14ac:dyDescent="0.25">
@@ -8576,10 +8309,10 @@
         <v>4</v>
       </c>
       <c r="R128" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="129" spans="1:28" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>312</v>
       </c>
@@ -8632,10 +8365,10 @@
         <v>1</v>
       </c>
       <c r="R129" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="130" spans="1:28" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="130" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>313</v>
       </c>
@@ -8688,10 +8421,10 @@
         <v>2</v>
       </c>
       <c r="R130" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="131" spans="1:28" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>314</v>
       </c>
@@ -8735,7 +8468,7 @@
         <v>0</v>
       </c>
       <c r="O131" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="P131" t="s">
         <v>18</v>
@@ -8744,10 +8477,10 @@
         <v>2</v>
       </c>
       <c r="R131" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="132" spans="1:28" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>316</v>
       </c>
@@ -8794,16 +8527,16 @@
         <v>21</v>
       </c>
       <c r="P132" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="Q132">
         <v>4</v>
       </c>
       <c r="R132" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="133" spans="1:28" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>317</v>
       </c>
@@ -8856,10 +8589,10 @@
         <v>5</v>
       </c>
       <c r="R133" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="134" spans="1:28" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>318</v>
       </c>
@@ -8912,10 +8645,10 @@
         <v>4</v>
       </c>
       <c r="R134" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="135" spans="1:28" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>319</v>
       </c>
@@ -8959,7 +8692,7 @@
         <v>0</v>
       </c>
       <c r="O135" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="P135" t="s">
         <v>18</v>
@@ -8968,10 +8701,10 @@
         <v>5</v>
       </c>
       <c r="R135" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="136" spans="1:28" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="136" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>320</v>
       </c>
@@ -9024,10 +8757,10 @@
         <v>3</v>
       </c>
       <c r="R136" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="137" spans="1:28" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>321</v>
       </c>
@@ -9080,10 +8813,10 @@
         <v>2</v>
       </c>
       <c r="R137" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="138" spans="1:28" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="138" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>322</v>
       </c>
@@ -9127,29 +8860,19 @@
         <v>0</v>
       </c>
       <c r="O138" s="2" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="P138" s="2" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="Q138" s="2" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="R138" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="S138" s="2"/>
-      <c r="T138" s="2"/>
-      <c r="U138" s="2"/>
-      <c r="V138" s="2"/>
-      <c r="W138" s="2"/>
-      <c r="X138" s="2"/>
-      <c r="Y138" s="2"/>
-      <c r="Z138" s="2"/>
-      <c r="AA138" s="2"/>
-      <c r="AB138" s="2"/>
-    </row>
-    <row r="139" spans="1:28" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="139" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>323</v>
       </c>
@@ -9193,7 +8916,7 @@
         <v>0</v>
       </c>
       <c r="O139" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="P139" t="s">
         <v>19</v>
@@ -9202,10 +8925,10 @@
         <v>5</v>
       </c>
       <c r="R139" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="140" spans="1:28" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="140" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>324</v>
       </c>
@@ -9258,10 +8981,10 @@
         <v>1</v>
       </c>
       <c r="R140" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="141" spans="1:28" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="141" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>326</v>
       </c>
@@ -9314,10 +9037,10 @@
         <v>4</v>
       </c>
       <c r="R141" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="142" spans="1:28" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>328</v>
       </c>
@@ -9370,10 +9093,10 @@
         <v>3</v>
       </c>
       <c r="R142" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="143" spans="1:28" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>329</v>
       </c>
@@ -9426,10 +9149,10 @@
         <v>4</v>
       </c>
       <c r="R143" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="144" spans="1:28" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="144" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>330</v>
       </c>
@@ -9482,10 +9205,10 @@
         <v>3</v>
       </c>
       <c r="R144" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="145" spans="1:28" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>331</v>
       </c>
@@ -9538,10 +9261,10 @@
         <v>4</v>
       </c>
       <c r="R145" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="146" spans="1:28" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>332</v>
       </c>
@@ -9594,10 +9317,10 @@
         <v>4</v>
       </c>
       <c r="R146" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="147" spans="1:28" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>333</v>
       </c>
@@ -9650,10 +9373,10 @@
         <v>4</v>
       </c>
       <c r="R147" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="148" spans="1:28" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>334</v>
       </c>
@@ -9706,10 +9429,10 @@
         <v>3</v>
       </c>
       <c r="R148" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="149" spans="1:28" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>335</v>
       </c>
@@ -9762,10 +9485,10 @@
         <v>4</v>
       </c>
       <c r="R149" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="150" spans="1:28" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>336</v>
       </c>
@@ -9818,10 +9541,10 @@
         <v>2</v>
       </c>
       <c r="R150" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="151" spans="1:28" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>337</v>
       </c>
@@ -9874,10 +9597,10 @@
         <v>1</v>
       </c>
       <c r="R151" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="152" spans="1:28" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>338</v>
       </c>
@@ -9930,10 +9653,10 @@
         <v>2</v>
       </c>
       <c r="R152" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="153" spans="1:28" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="153" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>339</v>
       </c>
@@ -9986,10 +9709,10 @@
         <v>1</v>
       </c>
       <c r="R153" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="154" spans="1:28" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>340</v>
       </c>
@@ -10042,10 +9765,10 @@
         <v>3</v>
       </c>
       <c r="R154" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="155" spans="1:28" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>341</v>
       </c>
@@ -10098,10 +9821,10 @@
         <v>2</v>
       </c>
       <c r="R155" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="156" spans="1:28" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="156" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>342</v>
       </c>
@@ -10154,10 +9877,10 @@
         <v>3</v>
       </c>
       <c r="R156" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="157" spans="1:28" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="157" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>343</v>
       </c>
@@ -10210,10 +9933,10 @@
         <v>4</v>
       </c>
       <c r="R157" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="158" spans="1:28" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>344</v>
       </c>
@@ -10266,10 +9989,10 @@
         <v>3</v>
       </c>
       <c r="R158" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="159" spans="1:28" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>345</v>
       </c>
@@ -10313,29 +10036,19 @@
         <v>0</v>
       </c>
       <c r="O159" s="2" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="P159" s="2" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="Q159" s="2" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="R159" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="S159" s="2"/>
-      <c r="T159" s="2"/>
-      <c r="U159" s="2"/>
-      <c r="V159" s="2"/>
-      <c r="W159" s="2"/>
-      <c r="X159" s="2"/>
-      <c r="Y159" s="2"/>
-      <c r="Z159" s="2"/>
-      <c r="AA159" s="2"/>
-      <c r="AB159" s="2"/>
-    </row>
-    <row r="160" spans="1:28" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>346</v>
       </c>
@@ -10388,7 +10101,7 @@
         <v>4</v>
       </c>
       <c r="R160" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
     </row>
     <row r="161" spans="1:18" x14ac:dyDescent="0.25">
@@ -10444,7 +10157,7 @@
         <v>3</v>
       </c>
       <c r="R161" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
     </row>
     <row r="162" spans="1:18" x14ac:dyDescent="0.25">
@@ -10500,7 +10213,7 @@
         <v>2</v>
       </c>
       <c r="R162" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
     </row>
     <row r="163" spans="1:18" x14ac:dyDescent="0.25">
@@ -10556,7 +10269,7 @@
         <v>4</v>
       </c>
       <c r="R163" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
     <row r="164" spans="1:18" x14ac:dyDescent="0.25">
@@ -10612,7 +10325,7 @@
         <v>3</v>
       </c>
       <c r="R164" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
     </row>
     <row r="165" spans="1:18" x14ac:dyDescent="0.25">
@@ -10668,7 +10381,7 @@
         <v>1</v>
       </c>
       <c r="R165" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
     </row>
     <row r="166" spans="1:18" x14ac:dyDescent="0.25">
@@ -10724,7 +10437,7 @@
         <v>2</v>
       </c>
       <c r="R166" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="167" spans="1:18" x14ac:dyDescent="0.25">
@@ -10780,7 +10493,7 @@
         <v>1</v>
       </c>
       <c r="R167" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
     </row>
     <row r="168" spans="1:18" x14ac:dyDescent="0.25">
@@ -10836,7 +10549,7 @@
         <v>3</v>
       </c>
       <c r="R168" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
     </row>
     <row r="169" spans="1:18" x14ac:dyDescent="0.25">
@@ -10892,7 +10605,7 @@
         <v>2</v>
       </c>
       <c r="R169" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
     </row>
     <row r="170" spans="1:18" x14ac:dyDescent="0.25">
@@ -10948,7 +10661,7 @@
         <v>2</v>
       </c>
       <c r="R170" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
     </row>
     <row r="171" spans="1:18" x14ac:dyDescent="0.25">
@@ -11004,7 +10717,7 @@
         <v>4</v>
       </c>
       <c r="R171" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
     </row>
     <row r="172" spans="1:18" x14ac:dyDescent="0.25">
@@ -11060,7 +10773,7 @@
         <v>4</v>
       </c>
       <c r="R172" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
     </row>
     <row r="173" spans="1:18" x14ac:dyDescent="0.25">
@@ -11116,7 +10829,7 @@
         <v>3</v>
       </c>
       <c r="R173" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
     </row>
     <row r="174" spans="1:18" x14ac:dyDescent="0.25">
@@ -11172,7 +10885,7 @@
         <v>3</v>
       </c>
       <c r="R174" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
     </row>
     <row r="175" spans="1:18" x14ac:dyDescent="0.25">
@@ -11228,7 +10941,7 @@
         <v>2</v>
       </c>
       <c r="R175" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
     </row>
     <row r="176" spans="1:18" x14ac:dyDescent="0.25">
@@ -11284,10 +10997,10 @@
         <v>4</v>
       </c>
       <c r="R176" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="177" spans="1:28" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="177" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>363</v>
       </c>
@@ -11340,10 +11053,10 @@
         <v>5</v>
       </c>
       <c r="R177" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="178" spans="1:28" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="178" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>364</v>
       </c>
@@ -11396,10 +11109,10 @@
         <v>5</v>
       </c>
       <c r="R178" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="179" spans="1:28" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="179" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
         <v>365</v>
       </c>
@@ -11443,29 +11156,19 @@
         <v>0</v>
       </c>
       <c r="O179" s="2" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="P179" s="2" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="Q179" s="2" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="R179" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="S179" s="2"/>
-      <c r="T179" s="2"/>
-      <c r="U179" s="2"/>
-      <c r="V179" s="2"/>
-      <c r="W179" s="2"/>
-      <c r="X179" s="2"/>
-      <c r="Y179" s="2"/>
-      <c r="Z179" s="2"/>
-      <c r="AA179" s="2"/>
-      <c r="AB179" s="2"/>
-    </row>
-    <row r="180" spans="1:28" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="180" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
         <v>365</v>
       </c>
@@ -11518,20 +11221,10 @@
         <v>3</v>
       </c>
       <c r="R180" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="S180" s="2"/>
-      <c r="T180" s="2"/>
-      <c r="U180" s="2"/>
-      <c r="V180" s="2"/>
-      <c r="W180" s="2"/>
-      <c r="X180" s="2"/>
-      <c r="Y180" s="2"/>
-      <c r="Z180" s="2"/>
-      <c r="AA180" s="2"/>
-      <c r="AB180" s="2"/>
-    </row>
-    <row r="181" spans="1:28" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="181" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>366</v>
       </c>
@@ -11584,10 +11277,10 @@
         <v>2</v>
       </c>
       <c r="R181" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="182" spans="1:28" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="182" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
         <v>367</v>
       </c>
@@ -11640,20 +11333,10 @@
         <v>2</v>
       </c>
       <c r="R182" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="S182" s="2"/>
-      <c r="T182" s="2"/>
-      <c r="U182" s="2"/>
-      <c r="V182" s="2"/>
-      <c r="W182" s="2"/>
-      <c r="X182" s="2"/>
-      <c r="Y182" s="2"/>
-      <c r="Z182" s="2"/>
-      <c r="AA182" s="2"/>
-      <c r="AB182" s="2"/>
-    </row>
-    <row r="183" spans="1:28" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="183" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
         <v>367</v>
       </c>
@@ -11706,20 +11389,10 @@
         <v>5</v>
       </c>
       <c r="R183" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="S183" s="2"/>
-      <c r="T183" s="2"/>
-      <c r="U183" s="2"/>
-      <c r="V183" s="2"/>
-      <c r="W183" s="2"/>
-      <c r="X183" s="2"/>
-      <c r="Y183" s="2"/>
-      <c r="Z183" s="2"/>
-      <c r="AA183" s="2"/>
-      <c r="AB183" s="2"/>
-    </row>
-    <row r="184" spans="1:28" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="184" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>368</v>
       </c>
@@ -11772,10 +11445,10 @@
         <v>3</v>
       </c>
       <c r="R184" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="185" spans="1:28" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="185" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>369</v>
       </c>
@@ -11828,10 +11501,10 @@
         <v>2</v>
       </c>
       <c r="R185" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="186" spans="1:28" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="186" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>370</v>
       </c>
@@ -11884,10 +11557,10 @@
         <v>3</v>
       </c>
       <c r="R186" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="187" spans="1:28" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="187" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>371</v>
       </c>
@@ -11940,10 +11613,10 @@
         <v>1</v>
       </c>
       <c r="R187" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="188" spans="1:28" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="188" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>372</v>
       </c>
@@ -11996,10 +11669,10 @@
         <v>4</v>
       </c>
       <c r="R188" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="189" spans="1:28" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="189" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>373</v>
       </c>
@@ -12052,10 +11725,10 @@
         <v>4</v>
       </c>
       <c r="R189" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="190" spans="1:28" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="190" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>374</v>
       </c>
@@ -12108,10 +11781,10 @@
         <v>4</v>
       </c>
       <c r="R190" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="191" spans="1:28" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="191" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>375</v>
       </c>
@@ -12164,10 +11837,10 @@
         <v>5</v>
       </c>
       <c r="R191" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="192" spans="1:28" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="192" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>376</v>
       </c>
@@ -12220,7 +11893,7 @@
         <v>2</v>
       </c>
       <c r="R192" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
     </row>
     <row r="193" spans="1:18" x14ac:dyDescent="0.25">
@@ -12276,7 +11949,7 @@
         <v>5</v>
       </c>
       <c r="R193" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
     </row>
     <row r="194" spans="1:18" x14ac:dyDescent="0.25">
@@ -12323,7 +11996,7 @@
         <v>0</v>
       </c>
       <c r="O194" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="P194" t="s">
         <v>19</v>
@@ -12332,7 +12005,7 @@
         <v>5</v>
       </c>
       <c r="R194" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
     </row>
     <row r="195" spans="1:18" x14ac:dyDescent="0.25">
@@ -12388,7 +12061,7 @@
         <v>4</v>
       </c>
       <c r="R195" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
     </row>
     <row r="196" spans="1:18" x14ac:dyDescent="0.25">
@@ -12444,7 +12117,7 @@
         <v>2</v>
       </c>
       <c r="R196" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
     </row>
     <row r="197" spans="1:18" x14ac:dyDescent="0.25">
@@ -12500,7 +12173,7 @@
         <v>2</v>
       </c>
       <c r="R197" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Struggling to clean up raw data so that it will aggregate nicely.
</commit_message>
<xml_diff>
--- a/raw-data-prep/raw_data/Debrief_TG.xlsx
+++ b/raw-data-prep/raw_data/Debrief_TG.xlsx
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>2.h</t>
-  </si>
-  <si>
-    <t>Game play affect distraction time</t>
   </si>
   <si>
     <t>Surprise</t>
@@ -738,6 +735,9 @@
   </si>
   <si>
     <t xml:space="preserve">To see if we assigned sterotypes based on our essay type </t>
+  </si>
+  <si>
+    <t>Game.affect.distraction</t>
   </si>
 </sst>
 </file>
@@ -1136,7 +1136,7 @@
   <dimension ref="A1:R197"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:AA1048576"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,16 +1188,16 @@
         <v>13</v>
       </c>
       <c r="O1" t="s">
+        <v>228</v>
+      </c>
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -1244,16 +1244,16 @@
         <v>0</v>
       </c>
       <c r="O2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q2">
         <v>2</v>
       </c>
       <c r="R2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -1300,16 +1300,16 @@
         <v>0</v>
       </c>
       <c r="O3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q3">
         <v>2</v>
       </c>
       <c r="R3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -1356,16 +1356,16 @@
         <v>0</v>
       </c>
       <c r="O4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q4">
         <v>2</v>
       </c>
       <c r="R4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -1412,16 +1412,16 @@
         <v>1</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q5" s="1">
         <v>3</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1468,16 +1468,16 @@
         <v>0</v>
       </c>
       <c r="O6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q6">
         <v>4</v>
       </c>
       <c r="R6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -1524,16 +1524,16 @@
         <v>0</v>
       </c>
       <c r="O7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q7">
         <v>3</v>
       </c>
       <c r="R7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -1580,16 +1580,16 @@
         <v>0</v>
       </c>
       <c r="O8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q8">
         <v>4</v>
       </c>
       <c r="R8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1636,16 +1636,16 @@
         <v>0</v>
       </c>
       <c r="O9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q9">
         <v>3</v>
       </c>
       <c r="R9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -1692,16 +1692,16 @@
         <v>0</v>
       </c>
       <c r="O10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q10">
         <v>4</v>
       </c>
       <c r="R10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -1748,16 +1748,16 @@
         <v>1</v>
       </c>
       <c r="O11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q11">
         <v>4</v>
       </c>
       <c r="R11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -1804,16 +1804,16 @@
         <v>0</v>
       </c>
       <c r="O12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q12">
         <v>4</v>
       </c>
       <c r="R12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -1860,16 +1860,16 @@
         <v>0</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q13" s="1">
         <v>2</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -1916,16 +1916,16 @@
         <v>0</v>
       </c>
       <c r="O14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q14">
         <v>4</v>
       </c>
       <c r="R14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -1972,16 +1972,16 @@
         <v>0</v>
       </c>
       <c r="O15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q15">
         <v>1</v>
       </c>
       <c r="R15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -2028,16 +2028,16 @@
         <v>0</v>
       </c>
       <c r="O16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q16">
         <v>2</v>
       </c>
       <c r="R16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -2084,16 +2084,16 @@
         <v>0</v>
       </c>
       <c r="O17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q17">
         <v>5</v>
       </c>
       <c r="R17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -2140,16 +2140,16 @@
         <v>0</v>
       </c>
       <c r="O18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q18">
         <v>5</v>
       </c>
       <c r="R18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -2196,16 +2196,16 @@
         <v>0</v>
       </c>
       <c r="O19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q19">
         <v>3</v>
       </c>
       <c r="R19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
@@ -2252,16 +2252,16 @@
         <v>0</v>
       </c>
       <c r="O20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q20">
         <v>4</v>
       </c>
       <c r="R20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -2308,16 +2308,16 @@
         <v>0</v>
       </c>
       <c r="O21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q21">
         <v>1</v>
       </c>
       <c r="R21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -2364,16 +2364,16 @@
         <v>0</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q22" s="1">
         <v>3</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -2420,16 +2420,16 @@
         <v>0</v>
       </c>
       <c r="O23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q23">
         <v>3</v>
       </c>
       <c r="R23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
@@ -2476,16 +2476,16 @@
         <v>0</v>
       </c>
       <c r="O24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q24">
         <v>1</v>
       </c>
       <c r="R24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
@@ -2532,16 +2532,16 @@
         <v>0</v>
       </c>
       <c r="O25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q25">
         <v>1</v>
       </c>
       <c r="R25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -2588,16 +2588,16 @@
         <v>0</v>
       </c>
       <c r="O26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q26">
         <v>2</v>
       </c>
       <c r="R26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
@@ -2644,16 +2644,16 @@
         <v>0</v>
       </c>
       <c r="O27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q27">
         <v>1</v>
       </c>
       <c r="R27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
@@ -2700,16 +2700,16 @@
         <v>0</v>
       </c>
       <c r="O28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q28">
         <v>4</v>
       </c>
       <c r="R28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
@@ -2756,16 +2756,16 @@
         <v>0</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q29" s="1">
         <v>4</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
@@ -2812,16 +2812,16 @@
         <v>0</v>
       </c>
       <c r="O30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q30">
         <v>2</v>
       </c>
       <c r="R30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
@@ -2868,16 +2868,16 @@
         <v>0</v>
       </c>
       <c r="O31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q31">
         <v>4</v>
       </c>
       <c r="R31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
@@ -2924,16 +2924,16 @@
         <v>0</v>
       </c>
       <c r="O32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q32">
         <v>4</v>
       </c>
       <c r="R32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
@@ -2980,16 +2980,16 @@
         <v>0</v>
       </c>
       <c r="O33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q33">
         <v>3</v>
       </c>
       <c r="R33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
@@ -3036,16 +3036,16 @@
         <v>0</v>
       </c>
       <c r="O34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q34">
         <v>2</v>
       </c>
       <c r="R34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
@@ -3092,16 +3092,16 @@
         <v>0</v>
       </c>
       <c r="O35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q35">
         <v>4</v>
       </c>
       <c r="R35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
@@ -3148,16 +3148,16 @@
         <v>0</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q36" s="1">
         <v>3</v>
       </c>
       <c r="R36" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -3204,16 +3204,16 @@
         <v>0</v>
       </c>
       <c r="O37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q37">
         <v>2</v>
       </c>
       <c r="R37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
@@ -3260,16 +3260,16 @@
         <v>0</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q38" s="1">
         <v>4</v>
       </c>
       <c r="R38" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
@@ -3316,16 +3316,16 @@
         <v>0</v>
       </c>
       <c r="O39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q39">
         <v>1</v>
       </c>
       <c r="R39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
@@ -3372,16 +3372,16 @@
         <v>0</v>
       </c>
       <c r="O40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q40">
         <v>1</v>
       </c>
       <c r="R40" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
@@ -3428,16 +3428,16 @@
         <v>0</v>
       </c>
       <c r="O41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P41" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q41">
         <v>1</v>
       </c>
       <c r="R41" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
@@ -3484,16 +3484,16 @@
         <v>0</v>
       </c>
       <c r="O42" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P42" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q42">
         <v>2</v>
       </c>
       <c r="R42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
@@ -3540,16 +3540,16 @@
         <v>1</v>
       </c>
       <c r="O43" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P43" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q43">
         <v>3</v>
       </c>
       <c r="R43" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
@@ -3596,16 +3596,16 @@
         <v>0</v>
       </c>
       <c r="O44" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P44" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q44">
         <v>2</v>
       </c>
       <c r="R44" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
@@ -3652,16 +3652,16 @@
         <v>0</v>
       </c>
       <c r="O45" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P45" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q45">
         <v>4</v>
       </c>
       <c r="R45" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
@@ -3675,10 +3675,10 @@
         <v>1</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F46" s="2">
         <v>0</v>
@@ -3708,16 +3708,16 @@
         <v>0</v>
       </c>
       <c r="O46" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P46" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q46" s="2">
         <v>2</v>
       </c>
       <c r="R46" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
@@ -3764,16 +3764,16 @@
         <v>0</v>
       </c>
       <c r="O47" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P47" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q47">
         <v>4</v>
       </c>
       <c r="R47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
@@ -3820,16 +3820,16 @@
         <v>0</v>
       </c>
       <c r="O48" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P48" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q48">
         <v>3</v>
       </c>
       <c r="R48" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
@@ -3876,16 +3876,16 @@
         <v>1</v>
       </c>
       <c r="O49" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P49" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q49">
         <v>3</v>
       </c>
       <c r="R49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
@@ -3908,10 +3908,10 @@
         <v>0</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I50" s="2">
         <v>0</v>
@@ -3920,28 +3920,28 @@
         <v>0</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M50" s="2">
         <v>1</v>
       </c>
       <c r="N50" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="O50" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P50" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q50" s="2">
         <v>3</v>
       </c>
       <c r="R50" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
@@ -3988,16 +3988,16 @@
         <v>0</v>
       </c>
       <c r="O51" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P51" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q51">
         <v>2</v>
       </c>
       <c r="R51" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
@@ -4044,16 +4044,16 @@
         <v>0</v>
       </c>
       <c r="O52" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P52" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q52">
         <v>3</v>
       </c>
       <c r="R52" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
@@ -4100,16 +4100,16 @@
         <v>0</v>
       </c>
       <c r="O53" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P53" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q53">
         <v>2</v>
       </c>
       <c r="R53" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
@@ -4156,16 +4156,16 @@
         <v>0</v>
       </c>
       <c r="O54" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P54" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q54">
         <v>3</v>
       </c>
       <c r="R54" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
@@ -4212,16 +4212,16 @@
         <v>0</v>
       </c>
       <c r="O55" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P55" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q55">
         <v>2</v>
       </c>
       <c r="R55" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
@@ -4268,16 +4268,16 @@
         <v>0</v>
       </c>
       <c r="O56" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P56" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q56" s="1">
         <v>1</v>
       </c>
       <c r="R56" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
@@ -4324,16 +4324,16 @@
         <v>0</v>
       </c>
       <c r="O57" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P57" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q57" s="1">
         <v>5</v>
       </c>
       <c r="R57" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
@@ -4380,16 +4380,16 @@
         <v>0</v>
       </c>
       <c r="O58" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P58" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q58">
         <v>3</v>
       </c>
       <c r="R58" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
@@ -4436,16 +4436,16 @@
         <v>0</v>
       </c>
       <c r="O59" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P59" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q59">
         <v>4</v>
       </c>
       <c r="R59" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
@@ -4492,16 +4492,16 @@
         <v>0</v>
       </c>
       <c r="O60" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P60" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q60">
         <v>1</v>
       </c>
       <c r="R60" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
@@ -4548,16 +4548,16 @@
         <v>0</v>
       </c>
       <c r="O61" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P61" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q61">
         <v>2</v>
       </c>
       <c r="R61" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
@@ -4604,16 +4604,16 @@
         <v>0</v>
       </c>
       <c r="O62" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P62" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q62" s="1">
         <v>3</v>
       </c>
       <c r="R62" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
@@ -4660,16 +4660,16 @@
         <v>0</v>
       </c>
       <c r="O63" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P63" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q63">
         <v>3</v>
       </c>
       <c r="R63" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
@@ -4716,16 +4716,16 @@
         <v>0</v>
       </c>
       <c r="O64" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P64" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q64">
         <v>5</v>
       </c>
       <c r="R64" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
@@ -4772,16 +4772,16 @@
         <v>0</v>
       </c>
       <c r="O65" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P65" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q65">
         <v>2</v>
       </c>
       <c r="R65" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.25">
@@ -4828,16 +4828,16 @@
         <v>0</v>
       </c>
       <c r="O66" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P66" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q66">
         <v>2</v>
       </c>
       <c r="R66" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.25">
@@ -4884,16 +4884,16 @@
         <v>1</v>
       </c>
       <c r="O67" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P67" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q67" s="1">
         <v>3</v>
       </c>
       <c r="R67" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
@@ -4940,16 +4940,16 @@
         <v>0</v>
       </c>
       <c r="O68" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P68" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q68">
         <v>4</v>
       </c>
       <c r="R68" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.25">
@@ -4996,16 +4996,16 @@
         <v>0</v>
       </c>
       <c r="O69" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P69" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q69">
         <v>3</v>
       </c>
       <c r="R69" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.25">
@@ -5052,16 +5052,16 @@
         <v>0</v>
       </c>
       <c r="O70" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P70" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q70">
         <v>1</v>
       </c>
       <c r="R70" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.25">
@@ -5108,16 +5108,16 @@
         <v>0</v>
       </c>
       <c r="O71" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P71" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q71">
         <v>4</v>
       </c>
       <c r="R71" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.25">
@@ -5164,16 +5164,16 @@
         <v>0</v>
       </c>
       <c r="O72" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P72" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q72">
         <v>4</v>
       </c>
       <c r="R72" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.25">
@@ -5220,16 +5220,16 @@
         <v>0</v>
       </c>
       <c r="O73" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P73" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q73">
         <v>1</v>
       </c>
       <c r="R73" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.25">
@@ -5276,16 +5276,16 @@
         <v>0</v>
       </c>
       <c r="O74" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P74" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q74">
         <v>4</v>
       </c>
       <c r="R74" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.25">
@@ -5332,16 +5332,16 @@
         <v>0</v>
       </c>
       <c r="O75" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P75" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q75">
         <v>2</v>
       </c>
       <c r="R75" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.25">
@@ -5388,16 +5388,16 @@
         <v>0</v>
       </c>
       <c r="O76" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P76" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q76">
         <v>2</v>
       </c>
       <c r="R76" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.25">
@@ -5444,16 +5444,16 @@
         <v>0</v>
       </c>
       <c r="O77" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P77" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q77">
         <v>2</v>
       </c>
       <c r="R77" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.25">
@@ -5500,16 +5500,16 @@
         <v>0</v>
       </c>
       <c r="O78" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P78" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q78">
         <v>2</v>
       </c>
       <c r="R78" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
@@ -5556,16 +5556,16 @@
         <v>0</v>
       </c>
       <c r="O79" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P79" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q79">
         <v>4</v>
       </c>
       <c r="R79" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.25">
@@ -5612,16 +5612,16 @@
         <v>0</v>
       </c>
       <c r="O80" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P80" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q80">
         <v>2</v>
       </c>
       <c r="R80" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.25">
@@ -5668,16 +5668,16 @@
         <v>0</v>
       </c>
       <c r="O81" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P81" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q81">
         <v>2</v>
       </c>
       <c r="R81" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.25">
@@ -5724,16 +5724,16 @@
         <v>0</v>
       </c>
       <c r="O82" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P82" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q82">
         <v>2</v>
       </c>
       <c r="R82" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.25">
@@ -5780,16 +5780,16 @@
         <v>0</v>
       </c>
       <c r="O83" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P83" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q83">
         <v>4</v>
       </c>
       <c r="R83" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.25">
@@ -5836,16 +5836,16 @@
         <v>0</v>
       </c>
       <c r="O84" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P84" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q84" s="1">
         <v>1</v>
       </c>
       <c r="R84" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.25">
@@ -5892,16 +5892,16 @@
         <v>1</v>
       </c>
       <c r="O85" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P85" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q85" s="1">
         <v>4</v>
       </c>
       <c r="R85" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.25">
@@ -5948,16 +5948,16 @@
         <v>1</v>
       </c>
       <c r="O86" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P86" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q86">
         <v>2</v>
       </c>
       <c r="R86" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.25">
@@ -6004,16 +6004,16 @@
         <v>0</v>
       </c>
       <c r="O87" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P87" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q87">
         <v>2</v>
       </c>
       <c r="R87" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.25">
@@ -6060,16 +6060,16 @@
         <v>0</v>
       </c>
       <c r="O88" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P88" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q88">
         <v>2</v>
       </c>
       <c r="R88" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.25">
@@ -6116,16 +6116,16 @@
         <v>0</v>
       </c>
       <c r="O89" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P89" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q89">
         <v>4</v>
       </c>
       <c r="R89" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.25">
@@ -6172,16 +6172,16 @@
         <v>0</v>
       </c>
       <c r="O90" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P90" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q90">
         <v>2</v>
       </c>
       <c r="R90" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.25">
@@ -6228,16 +6228,16 @@
         <v>0</v>
       </c>
       <c r="O91" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P91" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q91">
         <v>2</v>
       </c>
       <c r="R91" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.25">
@@ -6284,16 +6284,16 @@
         <v>0</v>
       </c>
       <c r="O92" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P92" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q92">
         <v>4</v>
       </c>
       <c r="R92" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.25">
@@ -6340,16 +6340,16 @@
         <v>0</v>
       </c>
       <c r="O93" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P93" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q93">
         <v>2</v>
       </c>
       <c r="R93" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.25">
@@ -6396,16 +6396,16 @@
         <v>0</v>
       </c>
       <c r="O94" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P94" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q94">
         <v>2</v>
       </c>
       <c r="R94" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.25">
@@ -6452,16 +6452,16 @@
         <v>0</v>
       </c>
       <c r="O95" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P95" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q95">
         <v>2</v>
       </c>
       <c r="R95" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.25">
@@ -6508,16 +6508,16 @@
         <v>0</v>
       </c>
       <c r="O96" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P96" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q96">
         <v>2</v>
       </c>
       <c r="R96" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.25">
@@ -6564,16 +6564,16 @@
         <v>0</v>
       </c>
       <c r="O97" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P97" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q97">
         <v>2</v>
       </c>
       <c r="R97" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.25">
@@ -6620,16 +6620,16 @@
         <v>0</v>
       </c>
       <c r="O98" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P98" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Q98">
         <v>2</v>
       </c>
       <c r="R98" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.25">
@@ -6676,16 +6676,16 @@
         <v>1</v>
       </c>
       <c r="O99" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P99" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Q99" s="1">
         <v>5</v>
       </c>
       <c r="R99" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.25">
@@ -6732,16 +6732,16 @@
         <v>0</v>
       </c>
       <c r="O100" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P100" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q100">
         <v>3</v>
       </c>
       <c r="R100" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.25">
@@ -6788,16 +6788,16 @@
         <v>0</v>
       </c>
       <c r="O101" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P101" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q101">
         <v>1</v>
       </c>
       <c r="R101" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.25">
@@ -6844,16 +6844,16 @@
         <v>0</v>
       </c>
       <c r="O102" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P102" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q102" s="1">
         <v>1</v>
       </c>
       <c r="R102" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.25">
@@ -6900,16 +6900,16 @@
         <v>0</v>
       </c>
       <c r="O103" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P103" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q103">
         <v>4</v>
       </c>
       <c r="R103" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.25">
@@ -6956,16 +6956,16 @@
         <v>0</v>
       </c>
       <c r="O104" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P104" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q104">
         <v>2</v>
       </c>
       <c r="R104" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.25">
@@ -7012,16 +7012,16 @@
         <v>0</v>
       </c>
       <c r="O105" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P105" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q105">
         <v>1</v>
       </c>
       <c r="R105" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.25">
@@ -7068,16 +7068,16 @@
         <v>0</v>
       </c>
       <c r="O106" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="P106" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q106" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="P106" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q106" s="2" t="s">
+      <c r="R106" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="R106" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.25">
@@ -7124,16 +7124,16 @@
         <v>0</v>
       </c>
       <c r="O107" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P107" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q107">
         <v>4</v>
       </c>
       <c r="R107" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="108" spans="1:18" x14ac:dyDescent="0.25">
@@ -7180,16 +7180,16 @@
         <v>0</v>
       </c>
       <c r="O108" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P108" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q108">
         <v>4</v>
       </c>
       <c r="R108" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.25">
@@ -7236,16 +7236,16 @@
         <v>0</v>
       </c>
       <c r="O109" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P109" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q109">
         <v>2</v>
       </c>
       <c r="R109" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.25">
@@ -7292,16 +7292,16 @@
         <v>0</v>
       </c>
       <c r="O110" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P110" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q110">
         <v>1</v>
       </c>
       <c r="R110" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="111" spans="1:18" x14ac:dyDescent="0.25">
@@ -7348,16 +7348,16 @@
         <v>1</v>
       </c>
       <c r="O111" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P111" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q111">
         <v>5</v>
       </c>
       <c r="R111" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.25">
@@ -7404,16 +7404,16 @@
         <v>0</v>
       </c>
       <c r="O112" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P112" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q112">
         <v>4</v>
       </c>
       <c r="R112" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.25">
@@ -7460,16 +7460,16 @@
         <v>0</v>
       </c>
       <c r="O113" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P113" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q113">
         <v>1</v>
       </c>
       <c r="R113" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="114" spans="1:18" x14ac:dyDescent="0.25">
@@ -7516,16 +7516,16 @@
         <v>0</v>
       </c>
       <c r="O114" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P114" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q114">
         <v>4</v>
       </c>
       <c r="R114" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="115" spans="1:18" x14ac:dyDescent="0.25">
@@ -7572,16 +7572,16 @@
         <v>0</v>
       </c>
       <c r="O115" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P115" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q115">
         <v>2</v>
       </c>
       <c r="R115" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.25">
@@ -7628,16 +7628,16 @@
         <v>0</v>
       </c>
       <c r="O116" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P116" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q116">
         <v>1</v>
       </c>
       <c r="R116" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.25">
@@ -7675,7 +7675,7 @@
         <v>0</v>
       </c>
       <c r="L117" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M117">
         <v>0</v>
@@ -7684,16 +7684,16 @@
         <v>0</v>
       </c>
       <c r="O117" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P117" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q117">
         <v>4</v>
       </c>
       <c r="R117" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.25">
@@ -7740,16 +7740,16 @@
         <v>0</v>
       </c>
       <c r="O118" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P118" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q118">
         <v>4</v>
       </c>
       <c r="R118" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.25">
@@ -7796,16 +7796,16 @@
         <v>0</v>
       </c>
       <c r="O119" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P119" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q119">
         <v>3</v>
       </c>
       <c r="R119" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="120" spans="1:18" x14ac:dyDescent="0.25">
@@ -7852,16 +7852,16 @@
         <v>0</v>
       </c>
       <c r="O120" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P120" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q120">
         <v>4</v>
       </c>
       <c r="R120" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="121" spans="1:18" x14ac:dyDescent="0.25">
@@ -7908,16 +7908,16 @@
         <v>0</v>
       </c>
       <c r="O121" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P121" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q121">
         <v>2</v>
       </c>
       <c r="R121" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="122" spans="1:18" x14ac:dyDescent="0.25">
@@ -7964,16 +7964,16 @@
         <v>0</v>
       </c>
       <c r="O122" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P122" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q122">
         <v>3</v>
       </c>
       <c r="R122" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="123" spans="1:18" x14ac:dyDescent="0.25">
@@ -8020,16 +8020,16 @@
         <v>0</v>
       </c>
       <c r="O123" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P123" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q123">
         <v>5</v>
       </c>
       <c r="R123" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="124" spans="1:18" x14ac:dyDescent="0.25">
@@ -8076,16 +8076,16 @@
         <v>0</v>
       </c>
       <c r="O124" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P124" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q124">
         <v>2</v>
       </c>
       <c r="R124" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="125" spans="1:18" x14ac:dyDescent="0.25">
@@ -8132,16 +8132,16 @@
         <v>0</v>
       </c>
       <c r="O125" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P125" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q125">
         <v>3</v>
       </c>
       <c r="R125" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="126" spans="1:18" x14ac:dyDescent="0.25">
@@ -8188,16 +8188,16 @@
         <v>0</v>
       </c>
       <c r="O126" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P126" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q126">
         <v>4</v>
       </c>
       <c r="R126" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="127" spans="1:18" x14ac:dyDescent="0.25">
@@ -8244,16 +8244,16 @@
         <v>0</v>
       </c>
       <c r="O127" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P127" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q127">
         <v>4</v>
       </c>
       <c r="R127" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="128" spans="1:18" x14ac:dyDescent="0.25">
@@ -8300,16 +8300,16 @@
         <v>0</v>
       </c>
       <c r="O128" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P128" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q128">
         <v>4</v>
       </c>
       <c r="R128" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="129" spans="1:18" x14ac:dyDescent="0.25">
@@ -8356,16 +8356,16 @@
         <v>0</v>
       </c>
       <c r="O129" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P129" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q129">
         <v>1</v>
       </c>
       <c r="R129" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="130" spans="1:18" x14ac:dyDescent="0.25">
@@ -8412,16 +8412,16 @@
         <v>0</v>
       </c>
       <c r="O130" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P130" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q130">
         <v>2</v>
       </c>
       <c r="R130" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="131" spans="1:18" x14ac:dyDescent="0.25">
@@ -8468,16 +8468,16 @@
         <v>0</v>
       </c>
       <c r="O131" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="P131" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q131">
         <v>2</v>
       </c>
       <c r="R131" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="132" spans="1:18" x14ac:dyDescent="0.25">
@@ -8524,16 +8524,16 @@
         <v>0</v>
       </c>
       <c r="O132" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P132" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Q132">
         <v>4</v>
       </c>
       <c r="R132" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="133" spans="1:18" x14ac:dyDescent="0.25">
@@ -8580,16 +8580,16 @@
         <v>0</v>
       </c>
       <c r="O133" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P133" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q133">
         <v>5</v>
       </c>
       <c r="R133" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="134" spans="1:18" x14ac:dyDescent="0.25">
@@ -8636,16 +8636,16 @@
         <v>0</v>
       </c>
       <c r="O134" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P134" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q134">
         <v>4</v>
       </c>
       <c r="R134" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="135" spans="1:18" x14ac:dyDescent="0.25">
@@ -8692,16 +8692,16 @@
         <v>0</v>
       </c>
       <c r="O135" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="P135" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q135">
         <v>5</v>
       </c>
       <c r="R135" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="136" spans="1:18" x14ac:dyDescent="0.25">
@@ -8748,16 +8748,16 @@
         <v>0</v>
       </c>
       <c r="O136" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P136" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q136">
         <v>3</v>
       </c>
       <c r="R136" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="137" spans="1:18" x14ac:dyDescent="0.25">
@@ -8804,16 +8804,16 @@
         <v>0</v>
       </c>
       <c r="O137" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P137" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q137">
         <v>2</v>
       </c>
       <c r="R137" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="138" spans="1:18" x14ac:dyDescent="0.25">
@@ -8860,16 +8860,16 @@
         <v>0</v>
       </c>
       <c r="O138" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="P138" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q138" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="P138" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q138" s="2" t="s">
+      <c r="R138" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="R138" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="139" spans="1:18" x14ac:dyDescent="0.25">
@@ -8916,16 +8916,16 @@
         <v>0</v>
       </c>
       <c r="O139" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="P139" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q139">
         <v>5</v>
       </c>
       <c r="R139" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="140" spans="1:18" x14ac:dyDescent="0.25">
@@ -8972,16 +8972,16 @@
         <v>0</v>
       </c>
       <c r="O140" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P140" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q140">
         <v>1</v>
       </c>
       <c r="R140" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="141" spans="1:18" x14ac:dyDescent="0.25">
@@ -9028,16 +9028,16 @@
         <v>0</v>
       </c>
       <c r="O141" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P141" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q141">
         <v>4</v>
       </c>
       <c r="R141" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="142" spans="1:18" x14ac:dyDescent="0.25">
@@ -9084,16 +9084,16 @@
         <v>0</v>
       </c>
       <c r="O142" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P142" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q142">
         <v>3</v>
       </c>
       <c r="R142" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="143" spans="1:18" x14ac:dyDescent="0.25">
@@ -9140,16 +9140,16 @@
         <v>0</v>
       </c>
       <c r="O143" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P143" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q143">
         <v>4</v>
       </c>
       <c r="R143" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="144" spans="1:18" x14ac:dyDescent="0.25">
@@ -9196,16 +9196,16 @@
         <v>0</v>
       </c>
       <c r="O144" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P144" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q144">
         <v>3</v>
       </c>
       <c r="R144" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="145" spans="1:18" x14ac:dyDescent="0.25">
@@ -9252,16 +9252,16 @@
         <v>0</v>
       </c>
       <c r="O145" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P145" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q145">
         <v>4</v>
       </c>
       <c r="R145" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="146" spans="1:18" x14ac:dyDescent="0.25">
@@ -9308,16 +9308,16 @@
         <v>0</v>
       </c>
       <c r="O146" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P146" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q146">
         <v>4</v>
       </c>
       <c r="R146" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="147" spans="1:18" x14ac:dyDescent="0.25">
@@ -9364,16 +9364,16 @@
         <v>0</v>
       </c>
       <c r="O147" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P147" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q147">
         <v>4</v>
       </c>
       <c r="R147" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="148" spans="1:18" x14ac:dyDescent="0.25">
@@ -9420,16 +9420,16 @@
         <v>0</v>
       </c>
       <c r="O148" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P148" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q148">
         <v>3</v>
       </c>
       <c r="R148" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="149" spans="1:18" x14ac:dyDescent="0.25">
@@ -9476,16 +9476,16 @@
         <v>0</v>
       </c>
       <c r="O149" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P149" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q149">
         <v>4</v>
       </c>
       <c r="R149" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="150" spans="1:18" x14ac:dyDescent="0.25">
@@ -9532,16 +9532,16 @@
         <v>0</v>
       </c>
       <c r="O150" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P150" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q150">
         <v>2</v>
       </c>
       <c r="R150" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="151" spans="1:18" x14ac:dyDescent="0.25">
@@ -9588,16 +9588,16 @@
         <v>1</v>
       </c>
       <c r="O151" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P151" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q151">
         <v>1</v>
       </c>
       <c r="R151" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="152" spans="1:18" x14ac:dyDescent="0.25">
@@ -9644,16 +9644,16 @@
         <v>0</v>
       </c>
       <c r="O152" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P152" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q152">
         <v>2</v>
       </c>
       <c r="R152" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="153" spans="1:18" x14ac:dyDescent="0.25">
@@ -9700,16 +9700,16 @@
         <v>0</v>
       </c>
       <c r="O153" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P153" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q153">
         <v>1</v>
       </c>
       <c r="R153" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="154" spans="1:18" x14ac:dyDescent="0.25">
@@ -9756,16 +9756,16 @@
         <v>0</v>
       </c>
       <c r="O154" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P154" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q154">
         <v>3</v>
       </c>
       <c r="R154" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="155" spans="1:18" x14ac:dyDescent="0.25">
@@ -9812,16 +9812,16 @@
         <v>0</v>
       </c>
       <c r="O155" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P155" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q155">
         <v>2</v>
       </c>
       <c r="R155" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="156" spans="1:18" x14ac:dyDescent="0.25">
@@ -9868,16 +9868,16 @@
         <v>0</v>
       </c>
       <c r="O156" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P156" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q156">
         <v>3</v>
       </c>
       <c r="R156" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="157" spans="1:18" x14ac:dyDescent="0.25">
@@ -9924,16 +9924,16 @@
         <v>0</v>
       </c>
       <c r="O157" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P157" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q157">
         <v>4</v>
       </c>
       <c r="R157" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="158" spans="1:18" x14ac:dyDescent="0.25">
@@ -9980,16 +9980,16 @@
         <v>0</v>
       </c>
       <c r="O158" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P158" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q158">
         <v>3</v>
       </c>
       <c r="R158" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="159" spans="1:18" x14ac:dyDescent="0.25">
@@ -10036,16 +10036,16 @@
         <v>0</v>
       </c>
       <c r="O159" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="P159" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q159" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="P159" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q159" s="2" t="s">
+      <c r="R159" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="R159" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="160" spans="1:18" x14ac:dyDescent="0.25">
@@ -10092,16 +10092,16 @@
         <v>0</v>
       </c>
       <c r="O160" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P160" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q160">
         <v>4</v>
       </c>
       <c r="R160" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="161" spans="1:18" x14ac:dyDescent="0.25">
@@ -10148,16 +10148,16 @@
         <v>0</v>
       </c>
       <c r="O161" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P161" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q161">
         <v>3</v>
       </c>
       <c r="R161" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="162" spans="1:18" x14ac:dyDescent="0.25">
@@ -10204,16 +10204,16 @@
         <v>0</v>
       </c>
       <c r="O162" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P162" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q162">
         <v>2</v>
       </c>
       <c r="R162" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="163" spans="1:18" x14ac:dyDescent="0.25">
@@ -10260,16 +10260,16 @@
         <v>0</v>
       </c>
       <c r="O163" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P163" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q163">
         <v>4</v>
       </c>
       <c r="R163" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="164" spans="1:18" x14ac:dyDescent="0.25">
@@ -10316,16 +10316,16 @@
         <v>0</v>
       </c>
       <c r="O164" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P164" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q164">
         <v>3</v>
       </c>
       <c r="R164" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="165" spans="1:18" x14ac:dyDescent="0.25">
@@ -10372,16 +10372,16 @@
         <v>0</v>
       </c>
       <c r="O165" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P165" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q165">
         <v>1</v>
       </c>
       <c r="R165" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="166" spans="1:18" x14ac:dyDescent="0.25">
@@ -10428,16 +10428,16 @@
         <v>0</v>
       </c>
       <c r="O166" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P166" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q166">
         <v>2</v>
       </c>
       <c r="R166" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="167" spans="1:18" x14ac:dyDescent="0.25">
@@ -10484,16 +10484,16 @@
         <v>0</v>
       </c>
       <c r="O167" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P167" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q167">
         <v>1</v>
       </c>
       <c r="R167" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="168" spans="1:18" x14ac:dyDescent="0.25">
@@ -10540,16 +10540,16 @@
         <v>0</v>
       </c>
       <c r="O168" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P168" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q168">
         <v>3</v>
       </c>
       <c r="R168" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="169" spans="1:18" x14ac:dyDescent="0.25">
@@ -10596,16 +10596,16 @@
         <v>0</v>
       </c>
       <c r="O169" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P169" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q169">
         <v>2</v>
       </c>
       <c r="R169" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="170" spans="1:18" x14ac:dyDescent="0.25">
@@ -10652,16 +10652,16 @@
         <v>0</v>
       </c>
       <c r="O170" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P170" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q170">
         <v>2</v>
       </c>
       <c r="R170" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="171" spans="1:18" x14ac:dyDescent="0.25">
@@ -10708,16 +10708,16 @@
         <v>0</v>
       </c>
       <c r="O171" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P171" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q171">
         <v>4</v>
       </c>
       <c r="R171" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="172" spans="1:18" x14ac:dyDescent="0.25">
@@ -10764,16 +10764,16 @@
         <v>0</v>
       </c>
       <c r="O172" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P172" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q172">
         <v>4</v>
       </c>
       <c r="R172" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="173" spans="1:18" x14ac:dyDescent="0.25">
@@ -10820,16 +10820,16 @@
         <v>0</v>
       </c>
       <c r="O173" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P173" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q173">
         <v>3</v>
       </c>
       <c r="R173" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="174" spans="1:18" x14ac:dyDescent="0.25">
@@ -10876,16 +10876,16 @@
         <v>0</v>
       </c>
       <c r="O174" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P174" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q174">
         <v>3</v>
       </c>
       <c r="R174" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="175" spans="1:18" x14ac:dyDescent="0.25">
@@ -10932,16 +10932,16 @@
         <v>0</v>
       </c>
       <c r="O175" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P175" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q175">
         <v>2</v>
       </c>
       <c r="R175" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="176" spans="1:18" x14ac:dyDescent="0.25">
@@ -10988,16 +10988,16 @@
         <v>1</v>
       </c>
       <c r="O176" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P176" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q176">
         <v>4</v>
       </c>
       <c r="R176" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="177" spans="1:18" x14ac:dyDescent="0.25">
@@ -11044,16 +11044,16 @@
         <v>0</v>
       </c>
       <c r="O177" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P177" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q177">
         <v>5</v>
       </c>
       <c r="R177" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="178" spans="1:18" x14ac:dyDescent="0.25">
@@ -11100,16 +11100,16 @@
         <v>0</v>
       </c>
       <c r="O178" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P178" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q178">
         <v>5</v>
       </c>
       <c r="R178" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="179" spans="1:18" x14ac:dyDescent="0.25">
@@ -11156,16 +11156,16 @@
         <v>0</v>
       </c>
       <c r="O179" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="P179" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q179" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="P179" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q179" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="R179" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="180" spans="1:18" x14ac:dyDescent="0.25">
@@ -11212,16 +11212,16 @@
         <v>0</v>
       </c>
       <c r="O180" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P180" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q180" s="2">
         <v>3</v>
       </c>
       <c r="R180" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="181" spans="1:18" x14ac:dyDescent="0.25">
@@ -11268,16 +11268,16 @@
         <v>0</v>
       </c>
       <c r="O181" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P181" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q181">
         <v>2</v>
       </c>
       <c r="R181" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="182" spans="1:18" x14ac:dyDescent="0.25">
@@ -11324,16 +11324,16 @@
         <v>0</v>
       </c>
       <c r="O182" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P182" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q182" s="2">
         <v>2</v>
       </c>
       <c r="R182" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="183" spans="1:18" x14ac:dyDescent="0.25">
@@ -11380,16 +11380,16 @@
         <v>0</v>
       </c>
       <c r="O183" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P183" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q183" s="2">
         <v>5</v>
       </c>
       <c r="R183" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="184" spans="1:18" x14ac:dyDescent="0.25">
@@ -11436,16 +11436,16 @@
         <v>0</v>
       </c>
       <c r="O184" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P184" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q184">
         <v>3</v>
       </c>
       <c r="R184" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="185" spans="1:18" x14ac:dyDescent="0.25">
@@ -11492,16 +11492,16 @@
         <v>0</v>
       </c>
       <c r="O185" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P185" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q185">
         <v>2</v>
       </c>
       <c r="R185" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="186" spans="1:18" x14ac:dyDescent="0.25">
@@ -11548,16 +11548,16 @@
         <v>0</v>
       </c>
       <c r="O186" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P186" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q186">
         <v>3</v>
       </c>
       <c r="R186" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="187" spans="1:18" x14ac:dyDescent="0.25">
@@ -11604,16 +11604,16 @@
         <v>0</v>
       </c>
       <c r="O187" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P187" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q187">
         <v>1</v>
       </c>
       <c r="R187" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="188" spans="1:18" x14ac:dyDescent="0.25">
@@ -11660,16 +11660,16 @@
         <v>1</v>
       </c>
       <c r="O188" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P188" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q188">
         <v>4</v>
       </c>
       <c r="R188" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="189" spans="1:18" x14ac:dyDescent="0.25">
@@ -11716,16 +11716,16 @@
         <v>0</v>
       </c>
       <c r="O189" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P189" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q189">
         <v>4</v>
       </c>
       <c r="R189" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="190" spans="1:18" x14ac:dyDescent="0.25">
@@ -11772,16 +11772,16 @@
         <v>0</v>
       </c>
       <c r="O190" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P190" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q190">
         <v>4</v>
       </c>
       <c r="R190" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="191" spans="1:18" x14ac:dyDescent="0.25">
@@ -11828,16 +11828,16 @@
         <v>0</v>
       </c>
       <c r="O191" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P191" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q191">
         <v>5</v>
       </c>
       <c r="R191" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="192" spans="1:18" x14ac:dyDescent="0.25">
@@ -11884,16 +11884,16 @@
         <v>0</v>
       </c>
       <c r="O192" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P192" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q192">
         <v>2</v>
       </c>
       <c r="R192" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="193" spans="1:18" x14ac:dyDescent="0.25">
@@ -11940,16 +11940,16 @@
         <v>0</v>
       </c>
       <c r="O193" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P193" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q193">
         <v>5</v>
       </c>
       <c r="R193" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="194" spans="1:18" x14ac:dyDescent="0.25">
@@ -11996,16 +11996,16 @@
         <v>0</v>
       </c>
       <c r="O194" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="P194" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q194">
         <v>5</v>
       </c>
       <c r="R194" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="195" spans="1:18" x14ac:dyDescent="0.25">
@@ -12052,16 +12052,16 @@
         <v>0</v>
       </c>
       <c r="O195" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P195" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q195">
         <v>4</v>
       </c>
       <c r="R195" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="196" spans="1:18" x14ac:dyDescent="0.25">
@@ -12108,16 +12108,16 @@
         <v>0</v>
       </c>
       <c r="O196" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P196" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q196">
         <v>2</v>
       </c>
       <c r="R196" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="197" spans="1:18" x14ac:dyDescent="0.25">
@@ -12164,16 +12164,16 @@
         <v>0</v>
       </c>
       <c r="O197" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P197" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q197">
         <v>2</v>
       </c>
       <c r="R197" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Move cell formatting to separate document. -Add some Hyunji data.
</commit_message>
<xml_diff>
--- a/raw-data-prep/raw_data/Debrief_TG.xlsx
+++ b/raw-data-prep/raw_data/Debrief_TG.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8235"/>
@@ -710,7 +710,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -789,11 +789,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -856,7 +858,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -891,7 +893,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1102,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R197"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,64 +1170,64 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>183</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2" t="s">
-        <v>147</v>
-      </c>
-      <c r="P2" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q2">
-        <v>2</v>
-      </c>
-      <c r="R2" t="s">
-        <v>16</v>
+      <c r="A2" s="4">
+        <v>168</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>1</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4">
+        <v>0</v>
+      </c>
+      <c r="L2" s="4">
+        <v>0</v>
+      </c>
+      <c r="M2" s="4">
+        <v>0</v>
+      </c>
+      <c r="N2" s="4">
+        <v>1</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>3</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1267,27 +1269,27 @@
         <v>0</v>
       </c>
       <c r="O3" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="P3" t="s">
-        <v>214</v>
+        <v>140</v>
       </c>
       <c r="Q3">
         <v>2</v>
       </c>
       <c r="R3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1299,7 +1301,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -1314,16 +1316,16 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4">
         <v>0</v>
       </c>
       <c r="O4" t="s">
-        <v>214</v>
+        <v>140</v>
       </c>
       <c r="P4" t="s">
         <v>214</v>
@@ -1332,63 +1334,63 @@
         <v>2</v>
       </c>
       <c r="R4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>185</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <v>0</v>
+      </c>
+      <c r="J5" s="5">
+        <v>0</v>
+      </c>
+      <c r="K5" s="5">
+        <v>0</v>
+      </c>
+      <c r="L5" s="5">
+        <v>1</v>
+      </c>
+      <c r="M5" s="5">
+        <v>0</v>
+      </c>
+      <c r="N5" s="5">
+        <v>0</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>2</v>
+      </c>
+      <c r="R5" s="5" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>168</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0</v>
-      </c>
-      <c r="K5" s="1">
-        <v>0</v>
-      </c>
-      <c r="L5" s="1">
-        <v>0</v>
-      </c>
-      <c r="M5" s="1">
-        <v>0</v>
-      </c>
-      <c r="N5" s="1">
-        <v>1</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>3</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1449,16 +1451,16 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1467,22 +1469,22 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7">
         <v>0</v>
       </c>
       <c r="K7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -1491,30 +1493,30 @@
         <v>0</v>
       </c>
       <c r="O7" t="s">
-        <v>140</v>
+        <v>213</v>
       </c>
       <c r="P7" t="s">
         <v>140</v>
       </c>
       <c r="Q7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1523,22 +1525,22 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -1547,16 +1549,16 @@
         <v>0</v>
       </c>
       <c r="O8" t="s">
-        <v>213</v>
+        <v>140</v>
       </c>
       <c r="P8" t="s">
         <v>140</v>
       </c>
       <c r="Q8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -2009,10 +2011,10 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -2021,7 +2023,7 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -2042,33 +2044,33 @@
         <v>0</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N17">
         <v>0</v>
       </c>
       <c r="O17" t="s">
-        <v>214</v>
+        <v>140</v>
       </c>
       <c r="P17" t="s">
-        <v>214</v>
+        <v>140</v>
       </c>
       <c r="Q17">
         <v>5</v>
       </c>
       <c r="R17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -2077,7 +2079,7 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -2098,25 +2100,25 @@
         <v>0</v>
       </c>
       <c r="L18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N18">
         <v>0</v>
       </c>
       <c r="O18" t="s">
-        <v>140</v>
+        <v>214</v>
       </c>
       <c r="P18" t="s">
-        <v>140</v>
+        <v>214</v>
       </c>
       <c r="Q18">
         <v>5</v>
       </c>
       <c r="R18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -12116,7 +12118,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R197"/>
+  <autoFilter ref="A1:R197">
+    <sortState ref="A2:R197">
+      <sortCondition ref="A1:A197"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>